<commit_message>
Back-end de tablas restantes
</commit_message>
<xml_diff>
--- a/Autorreporte/Requerimientos Reto Hackaton.xlsx
+++ b/Autorreporte/Requerimientos Reto Hackaton.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dm\Documentos\GitHub\hackatonmisionticunab\Autorreporte\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\diego\Documents\hackaton\hackatonmisionticunab\Autorreporte\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{119F1561-F2F1-4325-8DBE-7F00C0AF766E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9731DEE-77EF-49C7-AF9B-E2CCFFDE371F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{9B69EBA1-3CD1-4ED1-87D6-BACEB0337868}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{9B69EBA1-3CD1-4ED1-87D6-BACEB0337868}"/>
   </bookViews>
   <sheets>
     <sheet name="Listado de Requerimientos" sheetId="1" r:id="rId1"/>
@@ -527,20 +527,20 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -560,7 +560,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -859,67 +859,67 @@
   <dimension ref="A1:J144"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N6" sqref="N6"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="11.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="57.42578125" style="5" customWidth="1"/>
-    <col min="6" max="6" width="5.7109375" style="10" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.5703125" style="10" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="7.85546875" style="10" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12" style="10" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.140625" style="10"/>
+    <col min="1" max="1" width="11.81640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.26953125" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.54296875" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.81640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="57.453125" style="5" customWidth="1"/>
+    <col min="6" max="6" width="5.7265625" style="7" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.54296875" style="7" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.81640625" style="7" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12" style="7" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.1796875" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="62.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="8" t="s">
+    <row r="1" spans="1:10" ht="62.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8"/>
-      <c r="G1" s="8"/>
-      <c r="H1" s="8"/>
-      <c r="I1" s="8"/>
-      <c r="J1" s="8"/>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="7" t="s">
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
+      <c r="F1" s="9"/>
+      <c r="G1" s="9"/>
+      <c r="H1" s="9"/>
+      <c r="I1" s="9"/>
+      <c r="J1" s="9"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A2" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="9" t="s">
+      <c r="D2" s="11" t="s">
         <v>119</v>
       </c>
-      <c r="E2" s="9"/>
-      <c r="F2" s="9"/>
-      <c r="G2" s="9"/>
+      <c r="E2" s="11"/>
+      <c r="F2" s="11"/>
+      <c r="G2" s="11"/>
       <c r="H2" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="I2" s="11" t="s">
+      <c r="I2" s="8" t="s">
         <v>114</v>
       </c>
       <c r="J2" s="1" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="7"/>
-      <c r="B3" s="7"/>
-      <c r="C3" s="7"/>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A3" s="10"/>
+      <c r="B3" s="10"/>
+      <c r="C3" s="10"/>
       <c r="D3" s="1" t="s">
         <v>6</v>
       </c>
@@ -936,13 +936,13 @@
         <f>SUM(H4:H103)</f>
         <v>7660</v>
       </c>
-      <c r="I3" s="11"/>
+      <c r="I3" s="8"/>
       <c r="J3" s="1">
         <f>SUM(J4:J103)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A4" s="2">
         <v>1</v>
       </c>
@@ -958,25 +958,25 @@
       <c r="E4" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="F4" s="10">
+      <c r="F4" s="7">
         <v>30</v>
       </c>
-      <c r="G4" s="10">
-        <v>1</v>
-      </c>
-      <c r="H4" s="10">
+      <c r="G4" s="7">
+        <v>1</v>
+      </c>
+      <c r="H4" s="7">
         <f>F4*G4</f>
         <v>30</v>
       </c>
-      <c r="I4" s="10" t="s">
-        <v>117</v>
-      </c>
-      <c r="J4" s="10">
+      <c r="I4" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="J4" s="7">
         <f>IF(I4="Finalizado",H4,0)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A5" s="2">
         <v>2</v>
       </c>
@@ -992,25 +992,25 @@
       <c r="E5" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="F5" s="10">
+      <c r="F5" s="7">
         <v>30</v>
       </c>
-      <c r="G5" s="10">
-        <v>1</v>
-      </c>
-      <c r="H5" s="10">
+      <c r="G5" s="7">
+        <v>1</v>
+      </c>
+      <c r="H5" s="7">
         <f t="shared" ref="H5:H68" si="0">F5*G5</f>
         <v>30</v>
       </c>
-      <c r="I5" s="10" t="s">
-        <v>117</v>
-      </c>
-      <c r="J5" s="10">
+      <c r="I5" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="J5" s="7">
         <f t="shared" ref="J5:J68" si="1">IF(I5="Finalizado",H5,0)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A6" s="2">
         <v>3</v>
       </c>
@@ -1026,25 +1026,25 @@
       <c r="E6" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="F6" s="10">
+      <c r="F6" s="7">
         <v>30</v>
       </c>
-      <c r="G6" s="10">
-        <v>1</v>
-      </c>
-      <c r="H6" s="10">
+      <c r="G6" s="7">
+        <v>1</v>
+      </c>
+      <c r="H6" s="7">
         <f t="shared" si="0"/>
         <v>30</v>
       </c>
-      <c r="I6" s="10" t="s">
-        <v>117</v>
-      </c>
-      <c r="J6" s="10">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I6" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="J6" s="7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A7" s="2">
         <v>4</v>
       </c>
@@ -1060,25 +1060,25 @@
       <c r="E7" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="F7" s="10">
+      <c r="F7" s="7">
         <v>30</v>
       </c>
-      <c r="G7" s="10">
-        <v>1</v>
-      </c>
-      <c r="H7" s="10">
+      <c r="G7" s="7">
+        <v>1</v>
+      </c>
+      <c r="H7" s="7">
         <f t="shared" si="0"/>
         <v>30</v>
       </c>
-      <c r="I7" s="10" t="s">
-        <v>117</v>
-      </c>
-      <c r="J7" s="10">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I7" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="J7" s="7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A8" s="2">
         <v>5</v>
       </c>
@@ -1094,25 +1094,25 @@
       <c r="E8" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="F8" s="10">
+      <c r="F8" s="7">
         <v>30</v>
       </c>
-      <c r="G8" s="10">
-        <v>1</v>
-      </c>
-      <c r="H8" s="10">
+      <c r="G8" s="7">
+        <v>1</v>
+      </c>
+      <c r="H8" s="7">
         <f t="shared" si="0"/>
         <v>30</v>
       </c>
-      <c r="I8" s="10" t="s">
-        <v>117</v>
-      </c>
-      <c r="J8" s="10">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I8" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="J8" s="7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A9" s="2">
         <v>6</v>
       </c>
@@ -1128,25 +1128,25 @@
       <c r="E9" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="F9" s="10">
+      <c r="F9" s="7">
         <v>30</v>
       </c>
-      <c r="G9" s="10">
-        <v>1</v>
-      </c>
-      <c r="H9" s="10">
+      <c r="G9" s="7">
+        <v>1</v>
+      </c>
+      <c r="H9" s="7">
         <f t="shared" si="0"/>
         <v>30</v>
       </c>
-      <c r="I9" s="10" t="s">
-        <v>117</v>
-      </c>
-      <c r="J9" s="10">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I9" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="J9" s="7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A10" s="2">
         <v>7</v>
       </c>
@@ -1162,25 +1162,25 @@
       <c r="E10" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="F10" s="10">
+      <c r="F10" s="7">
         <v>30</v>
       </c>
-      <c r="G10" s="10">
-        <v>1</v>
-      </c>
-      <c r="H10" s="10">
+      <c r="G10" s="7">
+        <v>1</v>
+      </c>
+      <c r="H10" s="7">
         <f t="shared" si="0"/>
         <v>30</v>
       </c>
-      <c r="I10" s="10" t="s">
-        <v>117</v>
-      </c>
-      <c r="J10" s="10">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I10" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="J10" s="7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A11" s="2">
         <v>8</v>
       </c>
@@ -1196,25 +1196,25 @@
       <c r="E11" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="F11" s="10">
+      <c r="F11" s="7">
         <v>30</v>
       </c>
-      <c r="G11" s="10">
-        <v>1</v>
-      </c>
-      <c r="H11" s="10">
+      <c r="G11" s="7">
+        <v>1</v>
+      </c>
+      <c r="H11" s="7">
         <f t="shared" si="0"/>
         <v>30</v>
       </c>
-      <c r="I11" s="10" t="s">
-        <v>117</v>
-      </c>
-      <c r="J11" s="10">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I11" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="J11" s="7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A12" s="2">
         <v>9</v>
       </c>
@@ -1230,25 +1230,25 @@
       <c r="E12" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="F12" s="10">
+      <c r="F12" s="7">
         <v>30</v>
       </c>
-      <c r="G12" s="10">
-        <v>1</v>
-      </c>
-      <c r="H12" s="10">
+      <c r="G12" s="7">
+        <v>1</v>
+      </c>
+      <c r="H12" s="7">
         <f t="shared" si="0"/>
         <v>30</v>
       </c>
-      <c r="I12" s="10" t="s">
-        <v>117</v>
-      </c>
-      <c r="J12" s="10">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I12" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="J12" s="7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A13" s="2">
         <v>10</v>
       </c>
@@ -1264,25 +1264,25 @@
       <c r="E13" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="F13" s="10">
+      <c r="F13" s="7">
         <v>30</v>
       </c>
-      <c r="G13" s="10">
-        <v>1</v>
-      </c>
-      <c r="H13" s="10">
+      <c r="G13" s="7">
+        <v>1</v>
+      </c>
+      <c r="H13" s="7">
         <f t="shared" si="0"/>
         <v>30</v>
       </c>
-      <c r="I13" s="10" t="s">
-        <v>117</v>
-      </c>
-      <c r="J13" s="10">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I13" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="J13" s="7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A14" s="2">
         <v>11</v>
       </c>
@@ -1298,25 +1298,25 @@
       <c r="E14" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="F14" s="10">
+      <c r="F14" s="7">
         <v>30</v>
       </c>
-      <c r="G14" s="10">
-        <v>1</v>
-      </c>
-      <c r="H14" s="10">
+      <c r="G14" s="7">
+        <v>1</v>
+      </c>
+      <c r="H14" s="7">
         <f t="shared" si="0"/>
         <v>30</v>
       </c>
-      <c r="I14" s="10" t="s">
-        <v>117</v>
-      </c>
-      <c r="J14" s="10">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I14" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="J14" s="7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A15" s="2">
         <v>12</v>
       </c>
@@ -1332,25 +1332,25 @@
       <c r="E15" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="F15" s="10">
+      <c r="F15" s="7">
         <v>30</v>
       </c>
-      <c r="G15" s="10">
-        <v>1</v>
-      </c>
-      <c r="H15" s="10">
+      <c r="G15" s="7">
+        <v>1</v>
+      </c>
+      <c r="H15" s="7">
         <f t="shared" si="0"/>
         <v>30</v>
       </c>
-      <c r="I15" s="10" t="s">
-        <v>117</v>
-      </c>
-      <c r="J15" s="10">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I15" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="J15" s="7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A16" s="2">
         <v>13</v>
       </c>
@@ -1366,25 +1366,25 @@
       <c r="E16" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="F16" s="10">
+      <c r="F16" s="7">
         <v>30</v>
       </c>
-      <c r="G16" s="10">
-        <v>1</v>
-      </c>
-      <c r="H16" s="10">
+      <c r="G16" s="7">
+        <v>1</v>
+      </c>
+      <c r="H16" s="7">
         <f t="shared" si="0"/>
         <v>30</v>
       </c>
-      <c r="I16" s="10" t="s">
-        <v>117</v>
-      </c>
-      <c r="J16" s="10">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I16" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="J16" s="7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A17" s="2">
         <v>14</v>
       </c>
@@ -1400,25 +1400,25 @@
       <c r="E17" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="F17" s="10">
+      <c r="F17" s="7">
         <v>30</v>
       </c>
-      <c r="G17" s="10">
-        <v>1</v>
-      </c>
-      <c r="H17" s="10">
+      <c r="G17" s="7">
+        <v>1</v>
+      </c>
+      <c r="H17" s="7">
         <f t="shared" si="0"/>
         <v>30</v>
       </c>
-      <c r="I17" s="10" t="s">
-        <v>117</v>
-      </c>
-      <c r="J17" s="10">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I17" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="J17" s="7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A18" s="2">
         <v>15</v>
       </c>
@@ -1434,25 +1434,25 @@
       <c r="E18" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="F18" s="10">
+      <c r="F18" s="7">
         <v>30</v>
       </c>
-      <c r="G18" s="10">
-        <v>1</v>
-      </c>
-      <c r="H18" s="10">
+      <c r="G18" s="7">
+        <v>1</v>
+      </c>
+      <c r="H18" s="7">
         <f t="shared" si="0"/>
         <v>30</v>
       </c>
-      <c r="I18" s="10" t="s">
-        <v>117</v>
-      </c>
-      <c r="J18" s="10">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I18" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="J18" s="7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A19" s="2">
         <v>16</v>
       </c>
@@ -1468,25 +1468,25 @@
       <c r="E19" s="5" t="s">
         <v>89</v>
       </c>
-      <c r="F19" s="10">
+      <c r="F19" s="7">
         <v>30</v>
       </c>
-      <c r="G19" s="10">
-        <v>1</v>
-      </c>
-      <c r="H19" s="10">
+      <c r="G19" s="7">
+        <v>1</v>
+      </c>
+      <c r="H19" s="7">
         <f t="shared" si="0"/>
         <v>30</v>
       </c>
-      <c r="I19" s="10" t="s">
-        <v>117</v>
-      </c>
-      <c r="J19" s="10">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I19" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="J19" s="7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A20" s="2">
         <v>17</v>
       </c>
@@ -1502,25 +1502,25 @@
       <c r="E20" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="F20" s="10">
-        <v>10</v>
-      </c>
-      <c r="G20" s="10">
-        <v>1</v>
-      </c>
-      <c r="H20" s="10">
-        <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
-      <c r="I20" s="10" t="s">
-        <v>117</v>
-      </c>
-      <c r="J20" s="10">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F20" s="7">
+        <v>10</v>
+      </c>
+      <c r="G20" s="7">
+        <v>1</v>
+      </c>
+      <c r="H20" s="7">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="I20" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="J20" s="7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A21" s="2">
         <v>18</v>
       </c>
@@ -1536,25 +1536,25 @@
       <c r="E21" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="F21" s="10">
-        <v>10</v>
-      </c>
-      <c r="G21" s="10">
-        <v>1</v>
-      </c>
-      <c r="H21" s="10">
-        <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
-      <c r="I21" s="10" t="s">
-        <v>117</v>
-      </c>
-      <c r="J21" s="10">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F21" s="7">
+        <v>10</v>
+      </c>
+      <c r="G21" s="7">
+        <v>1</v>
+      </c>
+      <c r="H21" s="7">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="I21" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="J21" s="7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A22" s="2">
         <v>19</v>
       </c>
@@ -1570,25 +1570,25 @@
       <c r="E22" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="F22" s="10">
-        <v>10</v>
-      </c>
-      <c r="G22" s="10">
-        <v>1</v>
-      </c>
-      <c r="H22" s="10">
-        <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
-      <c r="I22" s="10" t="s">
-        <v>117</v>
-      </c>
-      <c r="J22" s="10">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F22" s="7">
+        <v>10</v>
+      </c>
+      <c r="G22" s="7">
+        <v>1</v>
+      </c>
+      <c r="H22" s="7">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="I22" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="J22" s="7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A23" s="2">
         <v>20</v>
       </c>
@@ -1604,25 +1604,25 @@
       <c r="E23" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="F23" s="10">
-        <v>10</v>
-      </c>
-      <c r="G23" s="10">
-        <v>1</v>
-      </c>
-      <c r="H23" s="10">
-        <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
-      <c r="I23" s="10" t="s">
-        <v>117</v>
-      </c>
-      <c r="J23" s="10">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F23" s="7">
+        <v>10</v>
+      </c>
+      <c r="G23" s="7">
+        <v>1</v>
+      </c>
+      <c r="H23" s="7">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="I23" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="J23" s="7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A24" s="2">
         <v>21</v>
       </c>
@@ -1638,25 +1638,25 @@
       <c r="E24" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="F24" s="10">
-        <v>10</v>
-      </c>
-      <c r="G24" s="10">
-        <v>1</v>
-      </c>
-      <c r="H24" s="10">
-        <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
-      <c r="I24" s="10" t="s">
-        <v>117</v>
-      </c>
-      <c r="J24" s="10">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F24" s="7">
+        <v>10</v>
+      </c>
+      <c r="G24" s="7">
+        <v>1</v>
+      </c>
+      <c r="H24" s="7">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="I24" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="J24" s="7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A25" s="2">
         <v>22</v>
       </c>
@@ -1672,25 +1672,25 @@
       <c r="E25" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="F25" s="10">
-        <v>10</v>
-      </c>
-      <c r="G25" s="10">
-        <v>1</v>
-      </c>
-      <c r="H25" s="10">
-        <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
-      <c r="I25" s="10" t="s">
-        <v>117</v>
-      </c>
-      <c r="J25" s="10">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F25" s="7">
+        <v>10</v>
+      </c>
+      <c r="G25" s="7">
+        <v>1</v>
+      </c>
+      <c r="H25" s="7">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="I25" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="J25" s="7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A26" s="2">
         <v>23</v>
       </c>
@@ -1706,25 +1706,25 @@
       <c r="E26" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="F26" s="10">
-        <v>10</v>
-      </c>
-      <c r="G26" s="10">
-        <v>1</v>
-      </c>
-      <c r="H26" s="10">
-        <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
-      <c r="I26" s="10" t="s">
-        <v>117</v>
-      </c>
-      <c r="J26" s="10">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F26" s="7">
+        <v>10</v>
+      </c>
+      <c r="G26" s="7">
+        <v>1</v>
+      </c>
+      <c r="H26" s="7">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="I26" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="J26" s="7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A27" s="2">
         <v>24</v>
       </c>
@@ -1740,25 +1740,25 @@
       <c r="E27" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="F27" s="10">
-        <v>10</v>
-      </c>
-      <c r="G27" s="10">
-        <v>1</v>
-      </c>
-      <c r="H27" s="10">
-        <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
-      <c r="I27" s="10" t="s">
-        <v>117</v>
-      </c>
-      <c r="J27" s="10">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F27" s="7">
+        <v>10</v>
+      </c>
+      <c r="G27" s="7">
+        <v>1</v>
+      </c>
+      <c r="H27" s="7">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="I27" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="J27" s="7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A28" s="2">
         <v>25</v>
       </c>
@@ -1774,25 +1774,25 @@
       <c r="E28" s="5" t="s">
         <v>120</v>
       </c>
-      <c r="F28" s="10">
-        <v>10</v>
-      </c>
-      <c r="G28" s="10">
-        <v>1</v>
-      </c>
-      <c r="H28" s="10">
-        <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
-      <c r="I28" s="10" t="s">
-        <v>117</v>
-      </c>
-      <c r="J28" s="10">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F28" s="7">
+        <v>10</v>
+      </c>
+      <c r="G28" s="7">
+        <v>1</v>
+      </c>
+      <c r="H28" s="7">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="I28" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="J28" s="7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A29" s="2">
         <v>26</v>
       </c>
@@ -1808,25 +1808,25 @@
       <c r="E29" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="F29" s="10">
-        <v>10</v>
-      </c>
-      <c r="G29" s="10">
-        <v>1</v>
-      </c>
-      <c r="H29" s="10">
-        <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
-      <c r="I29" s="10" t="s">
-        <v>117</v>
-      </c>
-      <c r="J29" s="10">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F29" s="7">
+        <v>10</v>
+      </c>
+      <c r="G29" s="7">
+        <v>1</v>
+      </c>
+      <c r="H29" s="7">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="I29" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="J29" s="7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A30" s="2">
         <v>27</v>
       </c>
@@ -1842,25 +1842,25 @@
       <c r="E30" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="F30" s="10">
-        <v>10</v>
-      </c>
-      <c r="G30" s="10">
-        <v>1</v>
-      </c>
-      <c r="H30" s="10">
-        <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
-      <c r="I30" s="10" t="s">
-        <v>117</v>
-      </c>
-      <c r="J30" s="10">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F30" s="7">
+        <v>10</v>
+      </c>
+      <c r="G30" s="7">
+        <v>1</v>
+      </c>
+      <c r="H30" s="7">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="I30" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="J30" s="7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A31" s="2">
         <v>28</v>
       </c>
@@ -1876,25 +1876,25 @@
       <c r="E31" s="5" t="s">
         <v>121</v>
       </c>
-      <c r="F31" s="10">
-        <v>10</v>
-      </c>
-      <c r="G31" s="10">
-        <v>1</v>
-      </c>
-      <c r="H31" s="10">
-        <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
-      <c r="I31" s="10" t="s">
-        <v>117</v>
-      </c>
-      <c r="J31" s="10">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F31" s="7">
+        <v>10</v>
+      </c>
+      <c r="G31" s="7">
+        <v>1</v>
+      </c>
+      <c r="H31" s="7">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="I31" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="J31" s="7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A32" s="2">
         <v>29</v>
       </c>
@@ -1910,25 +1910,25 @@
       <c r="E32" s="5" t="s">
         <v>122</v>
       </c>
-      <c r="F32" s="10">
-        <v>10</v>
-      </c>
-      <c r="G32" s="10">
-        <v>1</v>
-      </c>
-      <c r="H32" s="10">
-        <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
-      <c r="I32" s="10" t="s">
-        <v>117</v>
-      </c>
-      <c r="J32" s="10">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F32" s="7">
+        <v>10</v>
+      </c>
+      <c r="G32" s="7">
+        <v>1</v>
+      </c>
+      <c r="H32" s="7">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="I32" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="J32" s="7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A33" s="2">
         <v>30</v>
       </c>
@@ -1944,25 +1944,25 @@
       <c r="E33" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="F33" s="10">
-        <v>10</v>
-      </c>
-      <c r="G33" s="10">
-        <v>1</v>
-      </c>
-      <c r="H33" s="10">
-        <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
-      <c r="I33" s="10" t="s">
-        <v>117</v>
-      </c>
-      <c r="J33" s="10">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F33" s="7">
+        <v>10</v>
+      </c>
+      <c r="G33" s="7">
+        <v>1</v>
+      </c>
+      <c r="H33" s="7">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="I33" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="J33" s="7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A34" s="2">
         <v>31</v>
       </c>
@@ -1978,25 +1978,25 @@
       <c r="E34" s="5" t="s">
         <v>111</v>
       </c>
-      <c r="F34" s="10">
-        <v>10</v>
-      </c>
-      <c r="G34" s="10">
-        <v>1</v>
-      </c>
-      <c r="H34" s="10">
-        <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
-      <c r="I34" s="10" t="s">
-        <v>117</v>
-      </c>
-      <c r="J34" s="10">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F34" s="7">
+        <v>10</v>
+      </c>
+      <c r="G34" s="7">
+        <v>1</v>
+      </c>
+      <c r="H34" s="7">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="I34" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="J34" s="7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A35" s="2">
         <v>32</v>
       </c>
@@ -2012,25 +2012,25 @@
       <c r="E35" s="5" t="s">
         <v>112</v>
       </c>
-      <c r="F35" s="10">
-        <v>10</v>
-      </c>
-      <c r="G35" s="10">
-        <v>1</v>
-      </c>
-      <c r="H35" s="10">
-        <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
-      <c r="I35" s="10" t="s">
-        <v>117</v>
-      </c>
-      <c r="J35" s="10">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F35" s="7">
+        <v>10</v>
+      </c>
+      <c r="G35" s="7">
+        <v>1</v>
+      </c>
+      <c r="H35" s="7">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="I35" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="J35" s="7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A36" s="2">
         <v>33</v>
       </c>
@@ -2046,25 +2046,25 @@
       <c r="E36" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="F36" s="10">
-        <v>10</v>
-      </c>
-      <c r="G36" s="10">
-        <v>1</v>
-      </c>
-      <c r="H36" s="10">
-        <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
-      <c r="I36" s="10" t="s">
-        <v>117</v>
-      </c>
-      <c r="J36" s="10">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F36" s="7">
+        <v>10</v>
+      </c>
+      <c r="G36" s="7">
+        <v>1</v>
+      </c>
+      <c r="H36" s="7">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="I36" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="J36" s="7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A37" s="2">
         <v>34</v>
       </c>
@@ -2080,25 +2080,25 @@
       <c r="E37" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="F37" s="10">
-        <v>10</v>
-      </c>
-      <c r="G37" s="10">
-        <v>1</v>
-      </c>
-      <c r="H37" s="10">
-        <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
-      <c r="I37" s="10" t="s">
-        <v>117</v>
-      </c>
-      <c r="J37" s="10">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F37" s="7">
+        <v>10</v>
+      </c>
+      <c r="G37" s="7">
+        <v>1</v>
+      </c>
+      <c r="H37" s="7">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="I37" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="J37" s="7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A38" s="2">
         <v>35</v>
       </c>
@@ -2114,25 +2114,25 @@
       <c r="E38" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="F38" s="10">
-        <v>10</v>
-      </c>
-      <c r="G38" s="10">
-        <v>1</v>
-      </c>
-      <c r="H38" s="10">
-        <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
-      <c r="I38" s="10" t="s">
-        <v>117</v>
-      </c>
-      <c r="J38" s="10">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F38" s="7">
+        <v>10</v>
+      </c>
+      <c r="G38" s="7">
+        <v>1</v>
+      </c>
+      <c r="H38" s="7">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="I38" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="J38" s="7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A39" s="2">
         <v>36</v>
       </c>
@@ -2148,25 +2148,25 @@
       <c r="E39" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="F39" s="10">
-        <v>10</v>
-      </c>
-      <c r="G39" s="10">
-        <v>1</v>
-      </c>
-      <c r="H39" s="10">
-        <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
-      <c r="I39" s="10" t="s">
-        <v>117</v>
-      </c>
-      <c r="J39" s="10">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F39" s="7">
+        <v>10</v>
+      </c>
+      <c r="G39" s="7">
+        <v>1</v>
+      </c>
+      <c r="H39" s="7">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="I39" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="J39" s="7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A40" s="2">
         <v>37</v>
       </c>
@@ -2182,25 +2182,25 @@
       <c r="E40" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="F40" s="10">
-        <v>10</v>
-      </c>
-      <c r="G40" s="10">
-        <v>1</v>
-      </c>
-      <c r="H40" s="10">
-        <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
-      <c r="I40" s="10" t="s">
-        <v>117</v>
-      </c>
-      <c r="J40" s="10">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F40" s="7">
+        <v>10</v>
+      </c>
+      <c r="G40" s="7">
+        <v>1</v>
+      </c>
+      <c r="H40" s="7">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="I40" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="J40" s="7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A41" s="2">
         <v>38</v>
       </c>
@@ -2216,25 +2216,25 @@
       <c r="E41" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="F41" s="10">
-        <v>10</v>
-      </c>
-      <c r="G41" s="10">
-        <v>1</v>
-      </c>
-      <c r="H41" s="10">
-        <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
-      <c r="I41" s="10" t="s">
-        <v>117</v>
-      </c>
-      <c r="J41" s="10">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F41" s="7">
+        <v>10</v>
+      </c>
+      <c r="G41" s="7">
+        <v>1</v>
+      </c>
+      <c r="H41" s="7">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="I41" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="J41" s="7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A42" s="2">
         <v>39</v>
       </c>
@@ -2250,25 +2250,25 @@
       <c r="E42" s="5" t="s">
         <v>103</v>
       </c>
-      <c r="F42" s="10">
-        <v>10</v>
-      </c>
-      <c r="G42" s="10">
-        <v>1</v>
-      </c>
-      <c r="H42" s="10">
-        <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
-      <c r="I42" s="10" t="s">
-        <v>117</v>
-      </c>
-      <c r="J42" s="10">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F42" s="7">
+        <v>10</v>
+      </c>
+      <c r="G42" s="7">
+        <v>1</v>
+      </c>
+      <c r="H42" s="7">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="I42" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="J42" s="7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A43" s="2">
         <v>40</v>
       </c>
@@ -2284,25 +2284,25 @@
       <c r="E43" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="F43" s="10">
-        <v>10</v>
-      </c>
-      <c r="G43" s="10">
-        <v>1</v>
-      </c>
-      <c r="H43" s="10">
-        <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
-      <c r="I43" s="10" t="s">
-        <v>117</v>
-      </c>
-      <c r="J43" s="10">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F43" s="7">
+        <v>10</v>
+      </c>
+      <c r="G43" s="7">
+        <v>1</v>
+      </c>
+      <c r="H43" s="7">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="I43" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="J43" s="7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A44" s="2">
         <v>41</v>
       </c>
@@ -2318,25 +2318,25 @@
       <c r="E44" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="F44" s="10">
-        <v>10</v>
-      </c>
-      <c r="G44" s="10">
-        <v>1</v>
-      </c>
-      <c r="H44" s="10">
-        <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
-      <c r="I44" s="10" t="s">
-        <v>117</v>
-      </c>
-      <c r="J44" s="10">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F44" s="7">
+        <v>10</v>
+      </c>
+      <c r="G44" s="7">
+        <v>1</v>
+      </c>
+      <c r="H44" s="7">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="I44" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="J44" s="7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A45" s="2">
         <v>42</v>
       </c>
@@ -2352,25 +2352,25 @@
       <c r="E45" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="F45" s="10">
-        <v>10</v>
-      </c>
-      <c r="G45" s="10">
-        <v>1</v>
-      </c>
-      <c r="H45" s="10">
-        <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
-      <c r="I45" s="10" t="s">
-        <v>117</v>
-      </c>
-      <c r="J45" s="10">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F45" s="7">
+        <v>10</v>
+      </c>
+      <c r="G45" s="7">
+        <v>1</v>
+      </c>
+      <c r="H45" s="7">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="I45" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="J45" s="7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A46" s="2">
         <v>43</v>
       </c>
@@ -2386,25 +2386,25 @@
       <c r="E46" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="F46" s="10">
-        <v>10</v>
-      </c>
-      <c r="G46" s="10">
-        <v>1</v>
-      </c>
-      <c r="H46" s="10">
-        <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
-      <c r="I46" s="10" t="s">
-        <v>117</v>
-      </c>
-      <c r="J46" s="10">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F46" s="7">
+        <v>10</v>
+      </c>
+      <c r="G46" s="7">
+        <v>1</v>
+      </c>
+      <c r="H46" s="7">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="I46" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="J46" s="7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A47" s="2">
         <v>44</v>
       </c>
@@ -2420,25 +2420,25 @@
       <c r="E47" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="F47" s="10">
-        <v>10</v>
-      </c>
-      <c r="G47" s="10">
-        <v>1</v>
-      </c>
-      <c r="H47" s="10">
-        <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
-      <c r="I47" s="10" t="s">
-        <v>117</v>
-      </c>
-      <c r="J47" s="10">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F47" s="7">
+        <v>10</v>
+      </c>
+      <c r="G47" s="7">
+        <v>1</v>
+      </c>
+      <c r="H47" s="7">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="I47" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="J47" s="7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A48" s="2">
         <v>45</v>
       </c>
@@ -2454,25 +2454,25 @@
       <c r="E48" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="F48" s="10">
-        <v>10</v>
-      </c>
-      <c r="G48" s="10">
-        <v>1</v>
-      </c>
-      <c r="H48" s="10">
-        <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
-      <c r="I48" s="10" t="s">
-        <v>117</v>
-      </c>
-      <c r="J48" s="10">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F48" s="7">
+        <v>10</v>
+      </c>
+      <c r="G48" s="7">
+        <v>1</v>
+      </c>
+      <c r="H48" s="7">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="I48" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="J48" s="7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A49" s="2">
         <v>46</v>
       </c>
@@ -2488,25 +2488,25 @@
       <c r="E49" s="5" t="s">
         <v>79</v>
       </c>
-      <c r="F49" s="10">
-        <v>10</v>
-      </c>
-      <c r="G49" s="10">
-        <v>1</v>
-      </c>
-      <c r="H49" s="10">
-        <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
-      <c r="I49" s="10" t="s">
-        <v>117</v>
-      </c>
-      <c r="J49" s="10">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F49" s="7">
+        <v>10</v>
+      </c>
+      <c r="G49" s="7">
+        <v>1</v>
+      </c>
+      <c r="H49" s="7">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="I49" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="J49" s="7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A50" s="2">
         <v>47</v>
       </c>
@@ -2522,25 +2522,25 @@
       <c r="E50" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="F50" s="10">
+      <c r="F50" s="7">
         <v>20</v>
       </c>
-      <c r="G50" s="10">
-        <v>1</v>
-      </c>
-      <c r="H50" s="10">
+      <c r="G50" s="7">
+        <v>1</v>
+      </c>
+      <c r="H50" s="7">
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
-      <c r="I50" s="10" t="s">
-        <v>117</v>
-      </c>
-      <c r="J50" s="10">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I50" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="J50" s="7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A51" s="2">
         <v>48</v>
       </c>
@@ -2556,25 +2556,25 @@
       <c r="E51" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="F51" s="10">
+      <c r="F51" s="7">
         <v>20</v>
       </c>
-      <c r="G51" s="10">
-        <v>1</v>
-      </c>
-      <c r="H51" s="10">
+      <c r="G51" s="7">
+        <v>1</v>
+      </c>
+      <c r="H51" s="7">
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
-      <c r="I51" s="10" t="s">
-        <v>117</v>
-      </c>
-      <c r="J51" s="10">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I51" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="J51" s="7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A52" s="2">
         <v>49</v>
       </c>
@@ -2590,25 +2590,25 @@
       <c r="E52" s="5" t="s">
         <v>107</v>
       </c>
-      <c r="F52" s="10">
+      <c r="F52" s="7">
         <v>20</v>
       </c>
-      <c r="G52" s="10">
-        <v>1</v>
-      </c>
-      <c r="H52" s="10">
+      <c r="G52" s="7">
+        <v>1</v>
+      </c>
+      <c r="H52" s="7">
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
-      <c r="I52" s="10" t="s">
-        <v>117</v>
-      </c>
-      <c r="J52" s="10">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I52" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="J52" s="7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A53" s="2">
         <v>50</v>
       </c>
@@ -2624,25 +2624,25 @@
       <c r="E53" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="F53" s="10">
+      <c r="F53" s="7">
         <v>20</v>
       </c>
-      <c r="G53" s="10">
-        <v>1</v>
-      </c>
-      <c r="H53" s="10">
+      <c r="G53" s="7">
+        <v>1</v>
+      </c>
+      <c r="H53" s="7">
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
-      <c r="I53" s="10" t="s">
-        <v>117</v>
-      </c>
-      <c r="J53" s="10">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I53" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="J53" s="7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A54" s="2">
         <v>51</v>
       </c>
@@ -2658,25 +2658,25 @@
       <c r="E54" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="F54" s="10">
+      <c r="F54" s="7">
         <v>20</v>
       </c>
-      <c r="G54" s="10">
-        <v>1</v>
-      </c>
-      <c r="H54" s="10">
+      <c r="G54" s="7">
+        <v>1</v>
+      </c>
+      <c r="H54" s="7">
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
-      <c r="I54" s="10" t="s">
-        <v>117</v>
-      </c>
-      <c r="J54" s="10">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I54" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="J54" s="7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A55" s="2">
         <v>52</v>
       </c>
@@ -2692,25 +2692,25 @@
       <c r="E55" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="F55" s="10">
+      <c r="F55" s="7">
         <v>20</v>
       </c>
-      <c r="G55" s="10">
-        <v>1</v>
-      </c>
-      <c r="H55" s="10">
+      <c r="G55" s="7">
+        <v>1</v>
+      </c>
+      <c r="H55" s="7">
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
-      <c r="I55" s="10" t="s">
-        <v>117</v>
-      </c>
-      <c r="J55" s="10">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I55" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="J55" s="7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A56" s="2">
         <v>53</v>
       </c>
@@ -2726,25 +2726,25 @@
       <c r="E56" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="F56" s="10">
+      <c r="F56" s="7">
         <v>20</v>
       </c>
-      <c r="G56" s="10">
-        <v>1</v>
-      </c>
-      <c r="H56" s="10">
+      <c r="G56" s="7">
+        <v>1</v>
+      </c>
+      <c r="H56" s="7">
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
-      <c r="I56" s="10" t="s">
-        <v>117</v>
-      </c>
-      <c r="J56" s="10">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I56" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="J56" s="7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A57" s="2">
         <v>54</v>
       </c>
@@ -2760,25 +2760,25 @@
       <c r="E57" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="F57" s="10">
+      <c r="F57" s="7">
         <v>20</v>
       </c>
-      <c r="G57" s="10">
-        <v>1</v>
-      </c>
-      <c r="H57" s="10">
+      <c r="G57" s="7">
+        <v>1</v>
+      </c>
+      <c r="H57" s="7">
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
-      <c r="I57" s="10" t="s">
-        <v>117</v>
-      </c>
-      <c r="J57" s="10">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I57" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="J57" s="7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A58" s="2">
         <v>55</v>
       </c>
@@ -2794,25 +2794,25 @@
       <c r="E58" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="F58" s="10">
+      <c r="F58" s="7">
         <v>20</v>
       </c>
-      <c r="G58" s="10">
-        <v>1</v>
-      </c>
-      <c r="H58" s="10">
+      <c r="G58" s="7">
+        <v>1</v>
+      </c>
+      <c r="H58" s="7">
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
-      <c r="I58" s="10" t="s">
-        <v>117</v>
-      </c>
-      <c r="J58" s="10">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I58" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="J58" s="7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A59" s="2">
         <v>56</v>
       </c>
@@ -2828,25 +2828,25 @@
       <c r="E59" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="F59" s="10">
-        <v>10</v>
-      </c>
-      <c r="G59" s="10">
-        <v>1</v>
-      </c>
-      <c r="H59" s="10">
-        <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
-      <c r="I59" s="10" t="s">
-        <v>117</v>
-      </c>
-      <c r="J59" s="10">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F59" s="7">
+        <v>10</v>
+      </c>
+      <c r="G59" s="7">
+        <v>1</v>
+      </c>
+      <c r="H59" s="7">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="I59" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="J59" s="7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A60" s="2">
         <v>57</v>
       </c>
@@ -2862,25 +2862,25 @@
       <c r="E60" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="F60" s="10">
-        <v>10</v>
-      </c>
-      <c r="G60" s="10">
-        <v>1</v>
-      </c>
-      <c r="H60" s="10">
-        <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
-      <c r="I60" s="10" t="s">
-        <v>117</v>
-      </c>
-      <c r="J60" s="10">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F60" s="7">
+        <v>10</v>
+      </c>
+      <c r="G60" s="7">
+        <v>1</v>
+      </c>
+      <c r="H60" s="7">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="I60" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="J60" s="7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A61" s="2">
         <v>58</v>
       </c>
@@ -2896,25 +2896,25 @@
       <c r="E61" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="F61" s="10">
-        <v>10</v>
-      </c>
-      <c r="G61" s="10">
-        <v>1</v>
-      </c>
-      <c r="H61" s="10">
-        <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
-      <c r="I61" s="10" t="s">
-        <v>117</v>
-      </c>
-      <c r="J61" s="10">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F61" s="7">
+        <v>10</v>
+      </c>
+      <c r="G61" s="7">
+        <v>1</v>
+      </c>
+      <c r="H61" s="7">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="I61" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="J61" s="7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A62" s="2">
         <v>59</v>
       </c>
@@ -2930,25 +2930,25 @@
       <c r="E62" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="F62" s="10">
-        <v>10</v>
-      </c>
-      <c r="G62" s="10">
-        <v>1</v>
-      </c>
-      <c r="H62" s="10">
-        <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
-      <c r="I62" s="10" t="s">
-        <v>117</v>
-      </c>
-      <c r="J62" s="10">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F62" s="7">
+        <v>10</v>
+      </c>
+      <c r="G62" s="7">
+        <v>1</v>
+      </c>
+      <c r="H62" s="7">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="I62" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="J62" s="7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A63" s="2">
         <v>60</v>
       </c>
@@ -2964,25 +2964,25 @@
       <c r="E63" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="F63" s="10">
-        <v>10</v>
-      </c>
-      <c r="G63" s="10">
-        <v>1</v>
-      </c>
-      <c r="H63" s="10">
-        <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
-      <c r="I63" s="10" t="s">
-        <v>117</v>
-      </c>
-      <c r="J63" s="10">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F63" s="7">
+        <v>10</v>
+      </c>
+      <c r="G63" s="7">
+        <v>1</v>
+      </c>
+      <c r="H63" s="7">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="I63" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="J63" s="7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A64" s="2">
         <v>61</v>
       </c>
@@ -2998,25 +2998,25 @@
       <c r="E64" s="5" t="s">
         <v>88</v>
       </c>
-      <c r="F64" s="10">
-        <v>10</v>
-      </c>
-      <c r="G64" s="10">
-        <v>1</v>
-      </c>
-      <c r="H64" s="10">
-        <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
-      <c r="I64" s="10" t="s">
-        <v>117</v>
-      </c>
-      <c r="J64" s="10">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="65" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F64" s="7">
+        <v>10</v>
+      </c>
+      <c r="G64" s="7">
+        <v>1</v>
+      </c>
+      <c r="H64" s="7">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="I64" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="J64" s="7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A65" s="2">
         <v>62</v>
       </c>
@@ -3032,25 +3032,25 @@
       <c r="E65" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="F65" s="10">
-        <v>10</v>
-      </c>
-      <c r="G65" s="10">
-        <v>1</v>
-      </c>
-      <c r="H65" s="10">
-        <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
-      <c r="I65" s="10" t="s">
-        <v>117</v>
-      </c>
-      <c r="J65" s="10">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="66" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F65" s="7">
+        <v>10</v>
+      </c>
+      <c r="G65" s="7">
+        <v>1</v>
+      </c>
+      <c r="H65" s="7">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="I65" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="J65" s="7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A66" s="2">
         <v>63</v>
       </c>
@@ -3066,25 +3066,25 @@
       <c r="E66" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="F66" s="10">
-        <v>10</v>
-      </c>
-      <c r="G66" s="10">
-        <v>1</v>
-      </c>
-      <c r="H66" s="10">
-        <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
-      <c r="I66" s="10" t="s">
-        <v>117</v>
-      </c>
-      <c r="J66" s="10">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F66" s="7">
+        <v>10</v>
+      </c>
+      <c r="G66" s="7">
+        <v>1</v>
+      </c>
+      <c r="H66" s="7">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="I66" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="J66" s="7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A67" s="2">
         <v>64</v>
       </c>
@@ -3100,25 +3100,25 @@
       <c r="E67" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="F67" s="10">
-        <v>10</v>
-      </c>
-      <c r="G67" s="10">
-        <v>1</v>
-      </c>
-      <c r="H67" s="10">
-        <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
-      <c r="I67" s="10" t="s">
-        <v>117</v>
-      </c>
-      <c r="J67" s="10">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F67" s="7">
+        <v>10</v>
+      </c>
+      <c r="G67" s="7">
+        <v>1</v>
+      </c>
+      <c r="H67" s="7">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="I67" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="J67" s="7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A68" s="2">
         <v>65</v>
       </c>
@@ -3134,25 +3134,25 @@
       <c r="E68" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="F68" s="10">
-        <v>10</v>
-      </c>
-      <c r="G68" s="10">
-        <v>1</v>
-      </c>
-      <c r="H68" s="10">
-        <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
-      <c r="I68" s="10" t="s">
-        <v>117</v>
-      </c>
-      <c r="J68" s="10">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F68" s="7">
+        <v>10</v>
+      </c>
+      <c r="G68" s="7">
+        <v>1</v>
+      </c>
+      <c r="H68" s="7">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="I68" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="J68" s="7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A69" s="2">
         <v>66</v>
       </c>
@@ -3168,25 +3168,25 @@
       <c r="E69" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="F69" s="10">
-        <v>10</v>
-      </c>
-      <c r="G69" s="10">
-        <v>1</v>
-      </c>
-      <c r="H69" s="10">
+      <c r="F69" s="7">
+        <v>10</v>
+      </c>
+      <c r="G69" s="7">
+        <v>1</v>
+      </c>
+      <c r="H69" s="7">
         <f t="shared" ref="H69:H103" si="2">F69*G69</f>
         <v>10</v>
       </c>
-      <c r="I69" s="10" t="s">
-        <v>117</v>
-      </c>
-      <c r="J69" s="10">
+      <c r="I69" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="J69" s="7">
         <f t="shared" ref="J69:J103" si="3">IF(I69="Finalizado",H69,0)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A70" s="2">
         <v>67</v>
       </c>
@@ -3202,25 +3202,25 @@
       <c r="E70" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="F70" s="10">
-        <v>10</v>
-      </c>
-      <c r="G70" s="10">
-        <v>1</v>
-      </c>
-      <c r="H70" s="10">
+      <c r="F70" s="7">
+        <v>10</v>
+      </c>
+      <c r="G70" s="7">
+        <v>1</v>
+      </c>
+      <c r="H70" s="7">
         <f t="shared" si="2"/>
         <v>10</v>
       </c>
-      <c r="I70" s="10" t="s">
-        <v>117</v>
-      </c>
-      <c r="J70" s="10">
+      <c r="I70" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="J70" s="7">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A71" s="2">
         <v>68</v>
       </c>
@@ -3236,25 +3236,25 @@
       <c r="E71" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="F71" s="10">
-        <v>10</v>
-      </c>
-      <c r="G71" s="10">
-        <v>1</v>
-      </c>
-      <c r="H71" s="10">
+      <c r="F71" s="7">
+        <v>10</v>
+      </c>
+      <c r="G71" s="7">
+        <v>1</v>
+      </c>
+      <c r="H71" s="7">
         <f t="shared" si="2"/>
         <v>10</v>
       </c>
-      <c r="I71" s="10" t="s">
-        <v>117</v>
-      </c>
-      <c r="J71" s="10">
+      <c r="I71" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="J71" s="7">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A72" s="2">
         <v>69</v>
       </c>
@@ -3270,25 +3270,25 @@
       <c r="E72" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="F72" s="10">
-        <v>10</v>
-      </c>
-      <c r="G72" s="10">
-        <v>1</v>
-      </c>
-      <c r="H72" s="10">
+      <c r="F72" s="7">
+        <v>10</v>
+      </c>
+      <c r="G72" s="7">
+        <v>1</v>
+      </c>
+      <c r="H72" s="7">
         <f t="shared" si="2"/>
         <v>10</v>
       </c>
-      <c r="I72" s="10" t="s">
-        <v>117</v>
-      </c>
-      <c r="J72" s="10">
+      <c r="I72" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="J72" s="7">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A73" s="2">
         <v>70</v>
       </c>
@@ -3304,25 +3304,25 @@
       <c r="E73" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="F73" s="10">
-        <v>10</v>
-      </c>
-      <c r="G73" s="10">
-        <v>1</v>
-      </c>
-      <c r="H73" s="10">
+      <c r="F73" s="7">
+        <v>10</v>
+      </c>
+      <c r="G73" s="7">
+        <v>1</v>
+      </c>
+      <c r="H73" s="7">
         <f t="shared" si="2"/>
         <v>10</v>
       </c>
-      <c r="I73" s="10" t="s">
-        <v>117</v>
-      </c>
-      <c r="J73" s="10">
+      <c r="I73" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="J73" s="7">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A74" s="2">
         <v>71</v>
       </c>
@@ -3338,25 +3338,25 @@
       <c r="E74" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="F74" s="10">
-        <v>10</v>
-      </c>
-      <c r="G74" s="10">
-        <v>1</v>
-      </c>
-      <c r="H74" s="10">
+      <c r="F74" s="7">
+        <v>10</v>
+      </c>
+      <c r="G74" s="7">
+        <v>1</v>
+      </c>
+      <c r="H74" s="7">
         <f t="shared" si="2"/>
         <v>10</v>
       </c>
-      <c r="I74" s="10" t="s">
-        <v>117</v>
-      </c>
-      <c r="J74" s="10">
+      <c r="I74" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="J74" s="7">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A75" s="2">
         <v>72</v>
       </c>
@@ -3372,25 +3372,25 @@
       <c r="E75" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="F75" s="10">
-        <v>10</v>
-      </c>
-      <c r="G75" s="10">
-        <v>1</v>
-      </c>
-      <c r="H75" s="10">
+      <c r="F75" s="7">
+        <v>10</v>
+      </c>
+      <c r="G75" s="7">
+        <v>1</v>
+      </c>
+      <c r="H75" s="7">
         <f t="shared" si="2"/>
         <v>10</v>
       </c>
-      <c r="I75" s="10" t="s">
-        <v>117</v>
-      </c>
-      <c r="J75" s="10">
+      <c r="I75" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="J75" s="7">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A76" s="2">
         <v>73</v>
       </c>
@@ -3406,25 +3406,25 @@
       <c r="E76" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="F76" s="10">
-        <v>10</v>
-      </c>
-      <c r="G76" s="10">
-        <v>1</v>
-      </c>
-      <c r="H76" s="10">
+      <c r="F76" s="7">
+        <v>10</v>
+      </c>
+      <c r="G76" s="7">
+        <v>1</v>
+      </c>
+      <c r="H76" s="7">
         <f t="shared" si="2"/>
         <v>10</v>
       </c>
-      <c r="I76" s="10" t="s">
-        <v>117</v>
-      </c>
-      <c r="J76" s="10">
+      <c r="I76" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="J76" s="7">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A77" s="2">
         <v>74</v>
       </c>
@@ -3440,25 +3440,25 @@
       <c r="E77" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="F77" s="10">
-        <v>10</v>
-      </c>
-      <c r="G77" s="10">
-        <v>1</v>
-      </c>
-      <c r="H77" s="10">
+      <c r="F77" s="7">
+        <v>10</v>
+      </c>
+      <c r="G77" s="7">
+        <v>1</v>
+      </c>
+      <c r="H77" s="7">
         <f t="shared" si="2"/>
         <v>10</v>
       </c>
-      <c r="I77" s="10" t="s">
-        <v>117</v>
-      </c>
-      <c r="J77" s="10">
+      <c r="I77" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="J77" s="7">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A78" s="2">
         <v>75</v>
       </c>
@@ -3474,25 +3474,25 @@
       <c r="E78" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="F78" s="10">
-        <v>10</v>
-      </c>
-      <c r="G78" s="10">
-        <v>1</v>
-      </c>
-      <c r="H78" s="10">
+      <c r="F78" s="7">
+        <v>10</v>
+      </c>
+      <c r="G78" s="7">
+        <v>1</v>
+      </c>
+      <c r="H78" s="7">
         <f t="shared" si="2"/>
         <v>10</v>
       </c>
-      <c r="I78" s="10" t="s">
-        <v>117</v>
-      </c>
-      <c r="J78" s="10">
+      <c r="I78" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="J78" s="7">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A79" s="2">
         <v>76</v>
       </c>
@@ -3508,25 +3508,25 @@
       <c r="E79" s="5" t="s">
         <v>110</v>
       </c>
-      <c r="F79" s="10">
+      <c r="F79" s="7">
         <v>90</v>
       </c>
-      <c r="G79" s="10">
+      <c r="G79" s="7">
         <v>34</v>
       </c>
-      <c r="H79" s="10">
+      <c r="H79" s="7">
         <f t="shared" si="2"/>
         <v>3060</v>
       </c>
-      <c r="I79" s="10" t="s">
-        <v>117</v>
-      </c>
-      <c r="J79" s="10">
+      <c r="I79" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="J79" s="7">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A80" s="2">
         <v>77</v>
       </c>
@@ -3542,25 +3542,25 @@
       <c r="E80" s="5" t="s">
         <v>86</v>
       </c>
-      <c r="F80" s="10">
+      <c r="F80" s="7">
         <v>90</v>
       </c>
-      <c r="G80" s="10">
-        <v>3</v>
-      </c>
-      <c r="H80" s="10">
+      <c r="G80" s="7">
+        <v>3</v>
+      </c>
+      <c r="H80" s="7">
         <f t="shared" si="2"/>
         <v>270</v>
       </c>
-      <c r="I80" s="10" t="s">
-        <v>117</v>
-      </c>
-      <c r="J80" s="10">
+      <c r="I80" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="J80" s="7">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
-    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A81" s="2">
         <v>78</v>
       </c>
@@ -3576,25 +3576,25 @@
       <c r="E81" s="5" t="s">
         <v>104</v>
       </c>
-      <c r="F81" s="10">
+      <c r="F81" s="7">
         <v>90</v>
       </c>
-      <c r="G81" s="10">
-        <v>3</v>
-      </c>
-      <c r="H81" s="10">
+      <c r="G81" s="7">
+        <v>3</v>
+      </c>
+      <c r="H81" s="7">
         <f t="shared" si="2"/>
         <v>270</v>
       </c>
-      <c r="I81" s="10" t="s">
-        <v>117</v>
-      </c>
-      <c r="J81" s="10">
+      <c r="I81" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="J81" s="7">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
-    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A82" s="2">
         <v>79</v>
       </c>
@@ -3610,25 +3610,25 @@
       <c r="E82" s="5" t="s">
         <v>90</v>
       </c>
-      <c r="F82" s="10">
+      <c r="F82" s="7">
         <v>90</v>
       </c>
-      <c r="G82" s="10">
-        <v>3</v>
-      </c>
-      <c r="H82" s="10">
+      <c r="G82" s="7">
+        <v>3</v>
+      </c>
+      <c r="H82" s="7">
         <f t="shared" si="2"/>
         <v>270</v>
       </c>
-      <c r="I82" s="10" t="s">
-        <v>117</v>
-      </c>
-      <c r="J82" s="10">
+      <c r="I82" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="J82" s="7">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A83" s="2">
         <v>80</v>
       </c>
@@ -3644,25 +3644,25 @@
       <c r="E83" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="F83" s="10">
-        <v>10</v>
-      </c>
-      <c r="G83" s="10">
+      <c r="F83" s="7">
+        <v>10</v>
+      </c>
+      <c r="G83" s="7">
         <v>5</v>
       </c>
-      <c r="H83" s="10">
+      <c r="H83" s="7">
         <f t="shared" si="2"/>
         <v>50</v>
       </c>
-      <c r="I83" s="10" t="s">
-        <v>117</v>
-      </c>
-      <c r="J83" s="10">
+      <c r="I83" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="J83" s="7">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A84" s="2">
         <v>81</v>
       </c>
@@ -3678,25 +3678,25 @@
       <c r="E84" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="F84" s="10">
-        <v>10</v>
-      </c>
-      <c r="G84" s="10">
+      <c r="F84" s="7">
+        <v>10</v>
+      </c>
+      <c r="G84" s="7">
         <v>5</v>
       </c>
-      <c r="H84" s="10">
+      <c r="H84" s="7">
         <f t="shared" si="2"/>
         <v>50</v>
       </c>
-      <c r="I84" s="10" t="s">
-        <v>117</v>
-      </c>
-      <c r="J84" s="10">
+      <c r="I84" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="J84" s="7">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
-    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A85" s="2">
         <v>82</v>
       </c>
@@ -3712,25 +3712,25 @@
       <c r="E85" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="F85" s="10">
-        <v>10</v>
-      </c>
-      <c r="G85" s="10">
+      <c r="F85" s="7">
+        <v>10</v>
+      </c>
+      <c r="G85" s="7">
         <v>21</v>
       </c>
-      <c r="H85" s="10">
+      <c r="H85" s="7">
         <f t="shared" si="2"/>
         <v>210</v>
       </c>
-      <c r="I85" s="10" t="s">
-        <v>117</v>
-      </c>
-      <c r="J85" s="10">
+      <c r="I85" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="J85" s="7">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A86" s="2">
         <v>83</v>
       </c>
@@ -3746,25 +3746,25 @@
       <c r="E86" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="F86" s="10">
-        <v>10</v>
-      </c>
-      <c r="G86" s="10">
+      <c r="F86" s="7">
+        <v>10</v>
+      </c>
+      <c r="G86" s="7">
         <v>21</v>
       </c>
-      <c r="H86" s="10">
+      <c r="H86" s="7">
         <f t="shared" si="2"/>
         <v>210</v>
       </c>
-      <c r="I86" s="10" t="s">
-        <v>117</v>
-      </c>
-      <c r="J86" s="10">
+      <c r="I86" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="J86" s="7">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
-    <row r="87" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A87" s="2">
         <v>84</v>
       </c>
@@ -3780,25 +3780,25 @@
       <c r="E87" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="F87" s="10">
-        <v>10</v>
-      </c>
-      <c r="G87" s="10">
+      <c r="F87" s="7">
+        <v>10</v>
+      </c>
+      <c r="G87" s="7">
         <v>21</v>
       </c>
-      <c r="H87" s="10">
+      <c r="H87" s="7">
         <f t="shared" si="2"/>
         <v>210</v>
       </c>
-      <c r="I87" s="10" t="s">
-        <v>117</v>
-      </c>
-      <c r="J87" s="10">
+      <c r="I87" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="J87" s="7">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
-    <row r="88" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A88" s="2">
         <v>85</v>
       </c>
@@ -3814,25 +3814,25 @@
       <c r="E88" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="F88" s="10">
+      <c r="F88" s="7">
         <v>60</v>
       </c>
-      <c r="G88" s="10">
-        <v>3</v>
-      </c>
-      <c r="H88" s="10">
+      <c r="G88" s="7">
+        <v>3</v>
+      </c>
+      <c r="H88" s="7">
         <f t="shared" si="2"/>
         <v>180</v>
       </c>
-      <c r="I88" s="10" t="s">
-        <v>117</v>
-      </c>
-      <c r="J88" s="10">
+      <c r="I88" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="J88" s="7">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
-    <row r="89" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A89" s="2">
         <v>86</v>
       </c>
@@ -3848,25 +3848,25 @@
       <c r="E89" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="F89" s="10">
+      <c r="F89" s="7">
         <v>60</v>
       </c>
-      <c r="G89" s="10">
-        <v>3</v>
-      </c>
-      <c r="H89" s="10">
+      <c r="G89" s="7">
+        <v>3</v>
+      </c>
+      <c r="H89" s="7">
         <f t="shared" si="2"/>
         <v>180</v>
       </c>
-      <c r="I89" s="10" t="s">
-        <v>117</v>
-      </c>
-      <c r="J89" s="10">
+      <c r="I89" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="J89" s="7">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
-    <row r="90" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A90" s="2">
         <v>87</v>
       </c>
@@ -3882,25 +3882,25 @@
       <c r="E90" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="F90" s="10">
+      <c r="F90" s="7">
         <v>60</v>
       </c>
-      <c r="G90" s="10">
-        <v>3</v>
-      </c>
-      <c r="H90" s="10">
+      <c r="G90" s="7">
+        <v>3</v>
+      </c>
+      <c r="H90" s="7">
         <f t="shared" si="2"/>
         <v>180</v>
       </c>
-      <c r="I90" s="10" t="s">
-        <v>117</v>
-      </c>
-      <c r="J90" s="10">
+      <c r="I90" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="J90" s="7">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
-    <row r="91" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A91" s="2">
         <v>88</v>
       </c>
@@ -3916,25 +3916,25 @@
       <c r="E91" s="5" t="s">
         <v>98</v>
       </c>
-      <c r="F91" s="10">
+      <c r="F91" s="7">
         <v>60</v>
       </c>
-      <c r="G91" s="10">
-        <v>3</v>
-      </c>
-      <c r="H91" s="10">
+      <c r="G91" s="7">
+        <v>3</v>
+      </c>
+      <c r="H91" s="7">
         <f t="shared" si="2"/>
         <v>180</v>
       </c>
-      <c r="I91" s="10" t="s">
-        <v>117</v>
-      </c>
-      <c r="J91" s="10">
+      <c r="I91" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="J91" s="7">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
-    <row r="92" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A92" s="2">
         <v>89</v>
       </c>
@@ -3950,25 +3950,25 @@
       <c r="E92" s="5" t="s">
         <v>99</v>
       </c>
-      <c r="F92" s="10">
+      <c r="F92" s="7">
         <v>60</v>
       </c>
-      <c r="G92" s="10">
-        <v>3</v>
-      </c>
-      <c r="H92" s="10">
+      <c r="G92" s="7">
+        <v>3</v>
+      </c>
+      <c r="H92" s="7">
         <f t="shared" si="2"/>
         <v>180</v>
       </c>
-      <c r="I92" s="10" t="s">
-        <v>117</v>
-      </c>
-      <c r="J92" s="10">
+      <c r="I92" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="J92" s="7">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
-    <row r="93" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A93" s="2">
         <v>90</v>
       </c>
@@ -3984,25 +3984,25 @@
       <c r="E93" s="5" t="s">
         <v>100</v>
       </c>
-      <c r="F93" s="10">
+      <c r="F93" s="7">
         <v>60</v>
       </c>
-      <c r="G93" s="10">
-        <v>3</v>
-      </c>
-      <c r="H93" s="10">
+      <c r="G93" s="7">
+        <v>3</v>
+      </c>
+      <c r="H93" s="7">
         <f t="shared" si="2"/>
         <v>180</v>
       </c>
-      <c r="I93" s="10" t="s">
-        <v>117</v>
-      </c>
-      <c r="J93" s="10">
+      <c r="I93" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="J93" s="7">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
-    <row r="94" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A94" s="2">
         <v>91</v>
       </c>
@@ -4018,25 +4018,25 @@
       <c r="E94" s="5" t="s">
         <v>101</v>
       </c>
-      <c r="F94" s="10">
+      <c r="F94" s="7">
         <v>60</v>
       </c>
-      <c r="G94" s="10">
-        <v>3</v>
-      </c>
-      <c r="H94" s="10">
+      <c r="G94" s="7">
+        <v>3</v>
+      </c>
+      <c r="H94" s="7">
         <f t="shared" si="2"/>
         <v>180</v>
       </c>
-      <c r="I94" s="10" t="s">
-        <v>117</v>
-      </c>
-      <c r="J94" s="10">
+      <c r="I94" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="J94" s="7">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
-    <row r="95" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A95" s="2">
         <v>92</v>
       </c>
@@ -4052,25 +4052,25 @@
       <c r="E95" s="5" t="s">
         <v>102</v>
       </c>
-      <c r="F95" s="10">
+      <c r="F95" s="7">
         <v>60</v>
       </c>
-      <c r="G95" s="10">
-        <v>3</v>
-      </c>
-      <c r="H95" s="10">
+      <c r="G95" s="7">
+        <v>3</v>
+      </c>
+      <c r="H95" s="7">
         <f t="shared" si="2"/>
         <v>180</v>
       </c>
-      <c r="I95" s="10" t="s">
-        <v>117</v>
-      </c>
-      <c r="J95" s="10">
+      <c r="I95" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="J95" s="7">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
-    <row r="96" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A96" s="2">
         <v>93</v>
       </c>
@@ -4086,25 +4086,25 @@
       <c r="E96" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="F96" s="10">
-        <v>10</v>
-      </c>
-      <c r="G96" s="10">
-        <v>3</v>
-      </c>
-      <c r="H96" s="10">
+      <c r="F96" s="7">
+        <v>10</v>
+      </c>
+      <c r="G96" s="7">
+        <v>3</v>
+      </c>
+      <c r="H96" s="7">
         <f t="shared" si="2"/>
         <v>30</v>
       </c>
-      <c r="I96" s="10" t="s">
-        <v>117</v>
-      </c>
-      <c r="J96" s="10">
+      <c r="I96" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="J96" s="7">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
-    <row r="97" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A97" s="2">
         <v>94</v>
       </c>
@@ -4120,25 +4120,25 @@
       <c r="E97" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="F97" s="10">
-        <v>10</v>
-      </c>
-      <c r="G97" s="10">
-        <v>3</v>
-      </c>
-      <c r="H97" s="10">
+      <c r="F97" s="7">
+        <v>10</v>
+      </c>
+      <c r="G97" s="7">
+        <v>3</v>
+      </c>
+      <c r="H97" s="7">
         <f t="shared" si="2"/>
         <v>30</v>
       </c>
-      <c r="I97" s="10" t="s">
-        <v>117</v>
-      </c>
-      <c r="J97" s="10">
+      <c r="I97" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="J97" s="7">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
-    <row r="98" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A98" s="2">
         <v>95</v>
       </c>
@@ -4154,25 +4154,25 @@
       <c r="E98" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="F98" s="10">
-        <v>10</v>
-      </c>
-      <c r="G98" s="10">
-        <v>3</v>
-      </c>
-      <c r="H98" s="10">
+      <c r="F98" s="7">
+        <v>10</v>
+      </c>
+      <c r="G98" s="7">
+        <v>3</v>
+      </c>
+      <c r="H98" s="7">
         <f t="shared" si="2"/>
         <v>30</v>
       </c>
-      <c r="I98" s="10" t="s">
-        <v>117</v>
-      </c>
-      <c r="J98" s="10">
+      <c r="I98" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="J98" s="7">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
-    <row r="99" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A99" s="2">
         <v>96</v>
       </c>
@@ -4188,25 +4188,25 @@
       <c r="E99" s="5" t="s">
         <v>92</v>
       </c>
-      <c r="F99" s="10">
-        <v>10</v>
-      </c>
-      <c r="G99" s="10">
+      <c r="F99" s="7">
+        <v>10</v>
+      </c>
+      <c r="G99" s="7">
         <v>5</v>
       </c>
-      <c r="H99" s="10">
+      <c r="H99" s="7">
         <f t="shared" si="2"/>
         <v>50</v>
       </c>
-      <c r="I99" s="10" t="s">
-        <v>117</v>
-      </c>
-      <c r="J99" s="10">
+      <c r="I99" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="J99" s="7">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
-    <row r="100" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A100" s="2">
         <v>97</v>
       </c>
@@ -4222,25 +4222,25 @@
       <c r="E100" s="5" t="s">
         <v>93</v>
       </c>
-      <c r="F100" s="10">
-        <v>10</v>
-      </c>
-      <c r="G100" s="10">
-        <v>3</v>
-      </c>
-      <c r="H100" s="10">
+      <c r="F100" s="7">
+        <v>10</v>
+      </c>
+      <c r="G100" s="7">
+        <v>3</v>
+      </c>
+      <c r="H100" s="7">
         <f t="shared" si="2"/>
         <v>30</v>
       </c>
-      <c r="I100" s="10" t="s">
-        <v>117</v>
-      </c>
-      <c r="J100" s="10">
+      <c r="I100" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="J100" s="7">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
-    <row r="101" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A101" s="2">
         <v>98</v>
       </c>
@@ -4256,25 +4256,25 @@
       <c r="E101" s="5" t="s">
         <v>94</v>
       </c>
-      <c r="F101" s="10">
-        <v>10</v>
-      </c>
-      <c r="G101" s="10">
-        <v>3</v>
-      </c>
-      <c r="H101" s="10">
+      <c r="F101" s="7">
+        <v>10</v>
+      </c>
+      <c r="G101" s="7">
+        <v>3</v>
+      </c>
+      <c r="H101" s="7">
         <f t="shared" si="2"/>
         <v>30</v>
       </c>
-      <c r="I101" s="10" t="s">
-        <v>117</v>
-      </c>
-      <c r="J101" s="10">
+      <c r="I101" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="J101" s="7">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
-    <row r="102" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A102" s="2">
         <v>99</v>
       </c>
@@ -4290,25 +4290,25 @@
       <c r="E102" s="5" t="s">
         <v>95</v>
       </c>
-      <c r="F102" s="10">
-        <v>10</v>
-      </c>
-      <c r="G102" s="10">
+      <c r="F102" s="7">
+        <v>10</v>
+      </c>
+      <c r="G102" s="7">
         <v>13</v>
       </c>
-      <c r="H102" s="10">
+      <c r="H102" s="7">
         <f t="shared" si="2"/>
         <v>130</v>
       </c>
-      <c r="I102" s="10" t="s">
-        <v>117</v>
-      </c>
-      <c r="J102" s="10">
+      <c r="I102" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="J102" s="7">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
-    <row r="103" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A103" s="2">
         <v>100</v>
       </c>
@@ -4324,28 +4324,28 @@
       <c r="E103" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="F103" s="10">
-        <v>10</v>
-      </c>
-      <c r="G103" s="10">
+      <c r="F103" s="7">
+        <v>10</v>
+      </c>
+      <c r="G103" s="7">
         <v>13</v>
       </c>
-      <c r="H103" s="10">
+      <c r="H103" s="7">
         <f t="shared" si="2"/>
         <v>130</v>
       </c>
-      <c r="I103" s="10" t="s">
-        <v>117</v>
-      </c>
-      <c r="J103" s="10">
+      <c r="I103" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="J103" s="7">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
-    <row r="104" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:10" x14ac:dyDescent="0.35">
       <c r="E104" s="4"/>
     </row>
-    <row r="144" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="144" spans="5:5" x14ac:dyDescent="0.35">
       <c r="E144" s="3"/>
     </row>
   </sheetData>
@@ -4388,19 +4388,19 @@
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>115</v>
       </c>

</xml_diff>

<commit_message>
Primer merge full Kat+K
</commit_message>
<xml_diff>
--- a/Autorreporte/Requerimientos Reto Hackaton.xlsx
+++ b/Autorreporte/Requerimientos Reto Hackaton.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dm\Documentos\GitHub\hackatonmisionticunab\Autorreporte\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/c12a3f875df349ba/coweb/hackatonmisionticunab/Autorreporte/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{119F1561-F2F1-4325-8DBE-7F00C0AF766E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="18" documentId="8_{119F1561-F2F1-4325-8DBE-7F00C0AF766E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A10878F8-29B4-4297-8062-FC8637B94231}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{9B69EBA1-3CD1-4ED1-87D6-BACEB0337868}"/>
+    <workbookView xWindow="828" yWindow="1356" windowWidth="20832" windowHeight="11004" xr2:uid="{9B69EBA1-3CD1-4ED1-87D6-BACEB0337868}"/>
   </bookViews>
   <sheets>
     <sheet name="Listado de Requerimientos" sheetId="1" r:id="rId1"/>
@@ -527,20 +527,20 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -560,7 +560,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -858,68 +858,68 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DCDFB87B-5724-4F51-B052-A66AC58FFB9B}">
   <dimension ref="A1:J144"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N6" sqref="N6"/>
+    <sheetView tabSelected="1" topLeftCell="A50" workbookViewId="0">
+      <selection activeCell="E65" sqref="E65"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="57.42578125" style="5" customWidth="1"/>
-    <col min="6" max="6" width="5.7109375" style="10" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.5703125" style="10" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="7.85546875" style="10" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12" style="10" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.140625" style="10"/>
+    <col min="1" max="1" width="11.88671875" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.5546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="57.44140625" style="5" customWidth="1"/>
+    <col min="6" max="6" width="5.6640625" style="7" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.5546875" style="7" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.88671875" style="7" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12" style="7" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.109375" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="62.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="8" t="s">
+    <row r="1" spans="1:10" ht="62.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8"/>
-      <c r="G1" s="8"/>
-      <c r="H1" s="8"/>
-      <c r="I1" s="8"/>
-      <c r="J1" s="8"/>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="7" t="s">
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
+      <c r="F1" s="9"/>
+      <c r="G1" s="9"/>
+      <c r="H1" s="9"/>
+      <c r="I1" s="9"/>
+      <c r="J1" s="9"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A2" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="9" t="s">
+      <c r="D2" s="11" t="s">
         <v>119</v>
       </c>
-      <c r="E2" s="9"/>
-      <c r="F2" s="9"/>
-      <c r="G2" s="9"/>
+      <c r="E2" s="11"/>
+      <c r="F2" s="11"/>
+      <c r="G2" s="11"/>
       <c r="H2" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="I2" s="11" t="s">
+      <c r="I2" s="8" t="s">
         <v>114</v>
       </c>
       <c r="J2" s="1" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="7"/>
-      <c r="B3" s="7"/>
-      <c r="C3" s="7"/>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A3" s="10"/>
+      <c r="B3" s="10"/>
+      <c r="C3" s="10"/>
       <c r="D3" s="1" t="s">
         <v>6</v>
       </c>
@@ -936,13 +936,13 @@
         <f>SUM(H4:H103)</f>
         <v>7660</v>
       </c>
-      <c r="I3" s="11"/>
+      <c r="I3" s="8"/>
       <c r="J3" s="1">
         <f>SUM(J4:J103)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" s="2">
         <v>1</v>
       </c>
@@ -958,25 +958,25 @@
       <c r="E4" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="F4" s="10">
+      <c r="F4" s="7">
         <v>30</v>
       </c>
-      <c r="G4" s="10">
-        <v>1</v>
-      </c>
-      <c r="H4" s="10">
+      <c r="G4" s="7">
+        <v>1</v>
+      </c>
+      <c r="H4" s="7">
         <f>F4*G4</f>
         <v>30</v>
       </c>
-      <c r="I4" s="10" t="s">
-        <v>117</v>
-      </c>
-      <c r="J4" s="10">
+      <c r="I4" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="J4" s="7">
         <f>IF(I4="Finalizado",H4,0)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" s="2">
         <v>2</v>
       </c>
@@ -992,25 +992,25 @@
       <c r="E5" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="F5" s="10">
+      <c r="F5" s="7">
         <v>30</v>
       </c>
-      <c r="G5" s="10">
-        <v>1</v>
-      </c>
-      <c r="H5" s="10">
+      <c r="G5" s="7">
+        <v>1</v>
+      </c>
+      <c r="H5" s="7">
         <f t="shared" ref="H5:H68" si="0">F5*G5</f>
         <v>30</v>
       </c>
-      <c r="I5" s="10" t="s">
-        <v>117</v>
-      </c>
-      <c r="J5" s="10">
+      <c r="I5" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="J5" s="7">
         <f t="shared" ref="J5:J68" si="1">IF(I5="Finalizado",H5,0)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" s="2">
         <v>3</v>
       </c>
@@ -1026,25 +1026,25 @@
       <c r="E6" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="F6" s="10">
+      <c r="F6" s="7">
         <v>30</v>
       </c>
-      <c r="G6" s="10">
-        <v>1</v>
-      </c>
-      <c r="H6" s="10">
+      <c r="G6" s="7">
+        <v>1</v>
+      </c>
+      <c r="H6" s="7">
         <f t="shared" si="0"/>
         <v>30</v>
       </c>
-      <c r="I6" s="10" t="s">
-        <v>117</v>
-      </c>
-      <c r="J6" s="10">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I6" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="J6" s="7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" s="2">
         <v>4</v>
       </c>
@@ -1060,25 +1060,25 @@
       <c r="E7" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="F7" s="10">
+      <c r="F7" s="7">
         <v>30</v>
       </c>
-      <c r="G7" s="10">
-        <v>1</v>
-      </c>
-      <c r="H7" s="10">
+      <c r="G7" s="7">
+        <v>1</v>
+      </c>
+      <c r="H7" s="7">
         <f t="shared" si="0"/>
         <v>30</v>
       </c>
-      <c r="I7" s="10" t="s">
-        <v>117</v>
-      </c>
-      <c r="J7" s="10">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I7" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="J7" s="7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" s="2">
         <v>5</v>
       </c>
@@ -1094,25 +1094,25 @@
       <c r="E8" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="F8" s="10">
+      <c r="F8" s="7">
         <v>30</v>
       </c>
-      <c r="G8" s="10">
-        <v>1</v>
-      </c>
-      <c r="H8" s="10">
+      <c r="G8" s="7">
+        <v>1</v>
+      </c>
+      <c r="H8" s="7">
         <f t="shared" si="0"/>
         <v>30</v>
       </c>
-      <c r="I8" s="10" t="s">
-        <v>117</v>
-      </c>
-      <c r="J8" s="10">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I8" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="J8" s="7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" s="2">
         <v>6</v>
       </c>
@@ -1128,25 +1128,25 @@
       <c r="E9" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="F9" s="10">
+      <c r="F9" s="7">
         <v>30</v>
       </c>
-      <c r="G9" s="10">
-        <v>1</v>
-      </c>
-      <c r="H9" s="10">
+      <c r="G9" s="7">
+        <v>1</v>
+      </c>
+      <c r="H9" s="7">
         <f t="shared" si="0"/>
         <v>30</v>
       </c>
-      <c r="I9" s="10" t="s">
-        <v>117</v>
-      </c>
-      <c r="J9" s="10">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I9" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="J9" s="7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" s="2">
         <v>7</v>
       </c>
@@ -1162,25 +1162,25 @@
       <c r="E10" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="F10" s="10">
+      <c r="F10" s="7">
         <v>30</v>
       </c>
-      <c r="G10" s="10">
-        <v>1</v>
-      </c>
-      <c r="H10" s="10">
+      <c r="G10" s="7">
+        <v>1</v>
+      </c>
+      <c r="H10" s="7">
         <f t="shared" si="0"/>
         <v>30</v>
       </c>
-      <c r="I10" s="10" t="s">
-        <v>117</v>
-      </c>
-      <c r="J10" s="10">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I10" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="J10" s="7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" s="2">
         <v>8</v>
       </c>
@@ -1196,25 +1196,25 @@
       <c r="E11" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="F11" s="10">
+      <c r="F11" s="7">
         <v>30</v>
       </c>
-      <c r="G11" s="10">
-        <v>1</v>
-      </c>
-      <c r="H11" s="10">
+      <c r="G11" s="7">
+        <v>1</v>
+      </c>
+      <c r="H11" s="7">
         <f t="shared" si="0"/>
         <v>30</v>
       </c>
-      <c r="I11" s="10" t="s">
-        <v>117</v>
-      </c>
-      <c r="J11" s="10">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I11" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="J11" s="7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" s="2">
         <v>9</v>
       </c>
@@ -1230,25 +1230,25 @@
       <c r="E12" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="F12" s="10">
+      <c r="F12" s="7">
         <v>30</v>
       </c>
-      <c r="G12" s="10">
-        <v>1</v>
-      </c>
-      <c r="H12" s="10">
+      <c r="G12" s="7">
+        <v>1</v>
+      </c>
+      <c r="H12" s="7">
         <f t="shared" si="0"/>
         <v>30</v>
       </c>
-      <c r="I12" s="10" t="s">
-        <v>117</v>
-      </c>
-      <c r="J12" s="10">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I12" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="J12" s="7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13" s="2">
         <v>10</v>
       </c>
@@ -1264,25 +1264,25 @@
       <c r="E13" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="F13" s="10">
+      <c r="F13" s="7">
         <v>30</v>
       </c>
-      <c r="G13" s="10">
-        <v>1</v>
-      </c>
-      <c r="H13" s="10">
+      <c r="G13" s="7">
+        <v>1</v>
+      </c>
+      <c r="H13" s="7">
         <f t="shared" si="0"/>
         <v>30</v>
       </c>
-      <c r="I13" s="10" t="s">
-        <v>117</v>
-      </c>
-      <c r="J13" s="10">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I13" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="J13" s="7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14" s="2">
         <v>11</v>
       </c>
@@ -1298,25 +1298,25 @@
       <c r="E14" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="F14" s="10">
+      <c r="F14" s="7">
         <v>30</v>
       </c>
-      <c r="G14" s="10">
-        <v>1</v>
-      </c>
-      <c r="H14" s="10">
+      <c r="G14" s="7">
+        <v>1</v>
+      </c>
+      <c r="H14" s="7">
         <f t="shared" si="0"/>
         <v>30</v>
       </c>
-      <c r="I14" s="10" t="s">
-        <v>117</v>
-      </c>
-      <c r="J14" s="10">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I14" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="J14" s="7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A15" s="2">
         <v>12</v>
       </c>
@@ -1332,25 +1332,25 @@
       <c r="E15" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="F15" s="10">
+      <c r="F15" s="7">
         <v>30</v>
       </c>
-      <c r="G15" s="10">
-        <v>1</v>
-      </c>
-      <c r="H15" s="10">
+      <c r="G15" s="7">
+        <v>1</v>
+      </c>
+      <c r="H15" s="7">
         <f t="shared" si="0"/>
         <v>30</v>
       </c>
-      <c r="I15" s="10" t="s">
-        <v>117</v>
-      </c>
-      <c r="J15" s="10">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I15" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="J15" s="7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A16" s="2">
         <v>13</v>
       </c>
@@ -1366,25 +1366,25 @@
       <c r="E16" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="F16" s="10">
+      <c r="F16" s="7">
         <v>30</v>
       </c>
-      <c r="G16" s="10">
-        <v>1</v>
-      </c>
-      <c r="H16" s="10">
+      <c r="G16" s="7">
+        <v>1</v>
+      </c>
+      <c r="H16" s="7">
         <f t="shared" si="0"/>
         <v>30</v>
       </c>
-      <c r="I16" s="10" t="s">
-        <v>117</v>
-      </c>
-      <c r="J16" s="10">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I16" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="J16" s="7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A17" s="2">
         <v>14</v>
       </c>
@@ -1400,25 +1400,25 @@
       <c r="E17" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="F17" s="10">
+      <c r="F17" s="7">
         <v>30</v>
       </c>
-      <c r="G17" s="10">
-        <v>1</v>
-      </c>
-      <c r="H17" s="10">
+      <c r="G17" s="7">
+        <v>1</v>
+      </c>
+      <c r="H17" s="7">
         <f t="shared" si="0"/>
         <v>30</v>
       </c>
-      <c r="I17" s="10" t="s">
-        <v>117</v>
-      </c>
-      <c r="J17" s="10">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I17" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="J17" s="7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A18" s="2">
         <v>15</v>
       </c>
@@ -1434,25 +1434,25 @@
       <c r="E18" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="F18" s="10">
+      <c r="F18" s="7">
         <v>30</v>
       </c>
-      <c r="G18" s="10">
-        <v>1</v>
-      </c>
-      <c r="H18" s="10">
+      <c r="G18" s="7">
+        <v>1</v>
+      </c>
+      <c r="H18" s="7">
         <f t="shared" si="0"/>
         <v>30</v>
       </c>
-      <c r="I18" s="10" t="s">
-        <v>117</v>
-      </c>
-      <c r="J18" s="10">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I18" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="J18" s="7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A19" s="2">
         <v>16</v>
       </c>
@@ -1468,25 +1468,25 @@
       <c r="E19" s="5" t="s">
         <v>89</v>
       </c>
-      <c r="F19" s="10">
+      <c r="F19" s="7">
         <v>30</v>
       </c>
-      <c r="G19" s="10">
-        <v>1</v>
-      </c>
-      <c r="H19" s="10">
+      <c r="G19" s="7">
+        <v>1</v>
+      </c>
+      <c r="H19" s="7">
         <f t="shared" si="0"/>
         <v>30</v>
       </c>
-      <c r="I19" s="10" t="s">
-        <v>117</v>
-      </c>
-      <c r="J19" s="10">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I19" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="J19" s="7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A20" s="2">
         <v>17</v>
       </c>
@@ -1502,25 +1502,25 @@
       <c r="E20" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="F20" s="10">
-        <v>10</v>
-      </c>
-      <c r="G20" s="10">
-        <v>1</v>
-      </c>
-      <c r="H20" s="10">
-        <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
-      <c r="I20" s="10" t="s">
-        <v>117</v>
-      </c>
-      <c r="J20" s="10">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F20" s="7">
+        <v>10</v>
+      </c>
+      <c r="G20" s="7">
+        <v>1</v>
+      </c>
+      <c r="H20" s="7">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="I20" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="J20" s="7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A21" s="2">
         <v>18</v>
       </c>
@@ -1536,25 +1536,25 @@
       <c r="E21" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="F21" s="10">
-        <v>10</v>
-      </c>
-      <c r="G21" s="10">
-        <v>1</v>
-      </c>
-      <c r="H21" s="10">
-        <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
-      <c r="I21" s="10" t="s">
-        <v>117</v>
-      </c>
-      <c r="J21" s="10">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F21" s="7">
+        <v>10</v>
+      </c>
+      <c r="G21" s="7">
+        <v>1</v>
+      </c>
+      <c r="H21" s="7">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="I21" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="J21" s="7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A22" s="2">
         <v>19</v>
       </c>
@@ -1570,25 +1570,25 @@
       <c r="E22" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="F22" s="10">
-        <v>10</v>
-      </c>
-      <c r="G22" s="10">
-        <v>1</v>
-      </c>
-      <c r="H22" s="10">
-        <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
-      <c r="I22" s="10" t="s">
-        <v>117</v>
-      </c>
-      <c r="J22" s="10">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F22" s="7">
+        <v>10</v>
+      </c>
+      <c r="G22" s="7">
+        <v>1</v>
+      </c>
+      <c r="H22" s="7">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="I22" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="J22" s="7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A23" s="2">
         <v>20</v>
       </c>
@@ -1604,25 +1604,25 @@
       <c r="E23" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="F23" s="10">
-        <v>10</v>
-      </c>
-      <c r="G23" s="10">
-        <v>1</v>
-      </c>
-      <c r="H23" s="10">
-        <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
-      <c r="I23" s="10" t="s">
-        <v>117</v>
-      </c>
-      <c r="J23" s="10">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F23" s="7">
+        <v>10</v>
+      </c>
+      <c r="G23" s="7">
+        <v>1</v>
+      </c>
+      <c r="H23" s="7">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="I23" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="J23" s="7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A24" s="2">
         <v>21</v>
       </c>
@@ -1638,25 +1638,25 @@
       <c r="E24" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="F24" s="10">
-        <v>10</v>
-      </c>
-      <c r="G24" s="10">
-        <v>1</v>
-      </c>
-      <c r="H24" s="10">
-        <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
-      <c r="I24" s="10" t="s">
-        <v>117</v>
-      </c>
-      <c r="J24" s="10">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F24" s="7">
+        <v>10</v>
+      </c>
+      <c r="G24" s="7">
+        <v>1</v>
+      </c>
+      <c r="H24" s="7">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="I24" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="J24" s="7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A25" s="2">
         <v>22</v>
       </c>
@@ -1672,25 +1672,25 @@
       <c r="E25" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="F25" s="10">
-        <v>10</v>
-      </c>
-      <c r="G25" s="10">
-        <v>1</v>
-      </c>
-      <c r="H25" s="10">
-        <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
-      <c r="I25" s="10" t="s">
-        <v>117</v>
-      </c>
-      <c r="J25" s="10">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F25" s="7">
+        <v>10</v>
+      </c>
+      <c r="G25" s="7">
+        <v>1</v>
+      </c>
+      <c r="H25" s="7">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="I25" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="J25" s="7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A26" s="2">
         <v>23</v>
       </c>
@@ -1706,25 +1706,25 @@
       <c r="E26" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="F26" s="10">
-        <v>10</v>
-      </c>
-      <c r="G26" s="10">
-        <v>1</v>
-      </c>
-      <c r="H26" s="10">
-        <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
-      <c r="I26" s="10" t="s">
-        <v>117</v>
-      </c>
-      <c r="J26" s="10">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F26" s="7">
+        <v>10</v>
+      </c>
+      <c r="G26" s="7">
+        <v>1</v>
+      </c>
+      <c r="H26" s="7">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="I26" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="J26" s="7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A27" s="2">
         <v>24</v>
       </c>
@@ -1740,25 +1740,25 @@
       <c r="E27" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="F27" s="10">
-        <v>10</v>
-      </c>
-      <c r="G27" s="10">
-        <v>1</v>
-      </c>
-      <c r="H27" s="10">
-        <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
-      <c r="I27" s="10" t="s">
-        <v>117</v>
-      </c>
-      <c r="J27" s="10">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F27" s="7">
+        <v>10</v>
+      </c>
+      <c r="G27" s="7">
+        <v>1</v>
+      </c>
+      <c r="H27" s="7">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="I27" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="J27" s="7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A28" s="2">
         <v>25</v>
       </c>
@@ -1774,25 +1774,25 @@
       <c r="E28" s="5" t="s">
         <v>120</v>
       </c>
-      <c r="F28" s="10">
-        <v>10</v>
-      </c>
-      <c r="G28" s="10">
-        <v>1</v>
-      </c>
-      <c r="H28" s="10">
-        <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
-      <c r="I28" s="10" t="s">
-        <v>117</v>
-      </c>
-      <c r="J28" s="10">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F28" s="7">
+        <v>10</v>
+      </c>
+      <c r="G28" s="7">
+        <v>1</v>
+      </c>
+      <c r="H28" s="7">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="I28" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="J28" s="7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A29" s="2">
         <v>26</v>
       </c>
@@ -1808,25 +1808,25 @@
       <c r="E29" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="F29" s="10">
-        <v>10</v>
-      </c>
-      <c r="G29" s="10">
-        <v>1</v>
-      </c>
-      <c r="H29" s="10">
-        <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
-      <c r="I29" s="10" t="s">
-        <v>117</v>
-      </c>
-      <c r="J29" s="10">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F29" s="7">
+        <v>10</v>
+      </c>
+      <c r="G29" s="7">
+        <v>1</v>
+      </c>
+      <c r="H29" s="7">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="I29" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="J29" s="7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A30" s="2">
         <v>27</v>
       </c>
@@ -1842,25 +1842,25 @@
       <c r="E30" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="F30" s="10">
-        <v>10</v>
-      </c>
-      <c r="G30" s="10">
-        <v>1</v>
-      </c>
-      <c r="H30" s="10">
-        <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
-      <c r="I30" s="10" t="s">
-        <v>117</v>
-      </c>
-      <c r="J30" s="10">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F30" s="7">
+        <v>10</v>
+      </c>
+      <c r="G30" s="7">
+        <v>1</v>
+      </c>
+      <c r="H30" s="7">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="I30" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="J30" s="7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A31" s="2">
         <v>28</v>
       </c>
@@ -1876,25 +1876,25 @@
       <c r="E31" s="5" t="s">
         <v>121</v>
       </c>
-      <c r="F31" s="10">
-        <v>10</v>
-      </c>
-      <c r="G31" s="10">
-        <v>1</v>
-      </c>
-      <c r="H31" s="10">
-        <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
-      <c r="I31" s="10" t="s">
-        <v>117</v>
-      </c>
-      <c r="J31" s="10">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F31" s="7">
+        <v>10</v>
+      </c>
+      <c r="G31" s="7">
+        <v>1</v>
+      </c>
+      <c r="H31" s="7">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="I31" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="J31" s="7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A32" s="2">
         <v>29</v>
       </c>
@@ -1910,25 +1910,25 @@
       <c r="E32" s="5" t="s">
         <v>122</v>
       </c>
-      <c r="F32" s="10">
-        <v>10</v>
-      </c>
-      <c r="G32" s="10">
-        <v>1</v>
-      </c>
-      <c r="H32" s="10">
-        <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
-      <c r="I32" s="10" t="s">
-        <v>117</v>
-      </c>
-      <c r="J32" s="10">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F32" s="7">
+        <v>10</v>
+      </c>
+      <c r="G32" s="7">
+        <v>1</v>
+      </c>
+      <c r="H32" s="7">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="I32" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="J32" s="7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A33" s="2">
         <v>30</v>
       </c>
@@ -1944,25 +1944,25 @@
       <c r="E33" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="F33" s="10">
-        <v>10</v>
-      </c>
-      <c r="G33" s="10">
-        <v>1</v>
-      </c>
-      <c r="H33" s="10">
-        <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
-      <c r="I33" s="10" t="s">
-        <v>117</v>
-      </c>
-      <c r="J33" s="10">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F33" s="7">
+        <v>10</v>
+      </c>
+      <c r="G33" s="7">
+        <v>1</v>
+      </c>
+      <c r="H33" s="7">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="I33" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="J33" s="7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A34" s="2">
         <v>31</v>
       </c>
@@ -1978,25 +1978,25 @@
       <c r="E34" s="5" t="s">
         <v>111</v>
       </c>
-      <c r="F34" s="10">
-        <v>10</v>
-      </c>
-      <c r="G34" s="10">
-        <v>1</v>
-      </c>
-      <c r="H34" s="10">
-        <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
-      <c r="I34" s="10" t="s">
-        <v>117</v>
-      </c>
-      <c r="J34" s="10">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F34" s="7">
+        <v>10</v>
+      </c>
+      <c r="G34" s="7">
+        <v>1</v>
+      </c>
+      <c r="H34" s="7">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="I34" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="J34" s="7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A35" s="2">
         <v>32</v>
       </c>
@@ -2012,25 +2012,25 @@
       <c r="E35" s="5" t="s">
         <v>112</v>
       </c>
-      <c r="F35" s="10">
-        <v>10</v>
-      </c>
-      <c r="G35" s="10">
-        <v>1</v>
-      </c>
-      <c r="H35" s="10">
-        <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
-      <c r="I35" s="10" t="s">
-        <v>117</v>
-      </c>
-      <c r="J35" s="10">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F35" s="7">
+        <v>10</v>
+      </c>
+      <c r="G35" s="7">
+        <v>1</v>
+      </c>
+      <c r="H35" s="7">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="I35" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="J35" s="7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A36" s="2">
         <v>33</v>
       </c>
@@ -2046,25 +2046,25 @@
       <c r="E36" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="F36" s="10">
-        <v>10</v>
-      </c>
-      <c r="G36" s="10">
-        <v>1</v>
-      </c>
-      <c r="H36" s="10">
-        <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
-      <c r="I36" s="10" t="s">
-        <v>117</v>
-      </c>
-      <c r="J36" s="10">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F36" s="7">
+        <v>10</v>
+      </c>
+      <c r="G36" s="7">
+        <v>1</v>
+      </c>
+      <c r="H36" s="7">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="I36" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="J36" s="7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A37" s="2">
         <v>34</v>
       </c>
@@ -2080,25 +2080,25 @@
       <c r="E37" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="F37" s="10">
-        <v>10</v>
-      </c>
-      <c r="G37" s="10">
-        <v>1</v>
-      </c>
-      <c r="H37" s="10">
-        <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
-      <c r="I37" s="10" t="s">
-        <v>117</v>
-      </c>
-      <c r="J37" s="10">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F37" s="7">
+        <v>10</v>
+      </c>
+      <c r="G37" s="7">
+        <v>1</v>
+      </c>
+      <c r="H37" s="7">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="I37" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="J37" s="7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A38" s="2">
         <v>35</v>
       </c>
@@ -2114,25 +2114,25 @@
       <c r="E38" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="F38" s="10">
-        <v>10</v>
-      </c>
-      <c r="G38" s="10">
-        <v>1</v>
-      </c>
-      <c r="H38" s="10">
-        <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
-      <c r="I38" s="10" t="s">
-        <v>117</v>
-      </c>
-      <c r="J38" s="10">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F38" s="7">
+        <v>10</v>
+      </c>
+      <c r="G38" s="7">
+        <v>1</v>
+      </c>
+      <c r="H38" s="7">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="I38" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="J38" s="7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A39" s="2">
         <v>36</v>
       </c>
@@ -2148,25 +2148,25 @@
       <c r="E39" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="F39" s="10">
-        <v>10</v>
-      </c>
-      <c r="G39" s="10">
-        <v>1</v>
-      </c>
-      <c r="H39" s="10">
-        <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
-      <c r="I39" s="10" t="s">
-        <v>117</v>
-      </c>
-      <c r="J39" s="10">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F39" s="7">
+        <v>10</v>
+      </c>
+      <c r="G39" s="7">
+        <v>1</v>
+      </c>
+      <c r="H39" s="7">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="I39" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="J39" s="7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A40" s="2">
         <v>37</v>
       </c>
@@ -2182,25 +2182,25 @@
       <c r="E40" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="F40" s="10">
-        <v>10</v>
-      </c>
-      <c r="G40" s="10">
-        <v>1</v>
-      </c>
-      <c r="H40" s="10">
-        <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
-      <c r="I40" s="10" t="s">
-        <v>117</v>
-      </c>
-      <c r="J40" s="10">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F40" s="7">
+        <v>10</v>
+      </c>
+      <c r="G40" s="7">
+        <v>1</v>
+      </c>
+      <c r="H40" s="7">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="I40" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="J40" s="7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A41" s="2">
         <v>38</v>
       </c>
@@ -2216,25 +2216,25 @@
       <c r="E41" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="F41" s="10">
-        <v>10</v>
-      </c>
-      <c r="G41" s="10">
-        <v>1</v>
-      </c>
-      <c r="H41" s="10">
-        <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
-      <c r="I41" s="10" t="s">
-        <v>117</v>
-      </c>
-      <c r="J41" s="10">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F41" s="7">
+        <v>10</v>
+      </c>
+      <c r="G41" s="7">
+        <v>1</v>
+      </c>
+      <c r="H41" s="7">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="I41" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="J41" s="7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A42" s="2">
         <v>39</v>
       </c>
@@ -2250,25 +2250,25 @@
       <c r="E42" s="5" t="s">
         <v>103</v>
       </c>
-      <c r="F42" s="10">
-        <v>10</v>
-      </c>
-      <c r="G42" s="10">
-        <v>1</v>
-      </c>
-      <c r="H42" s="10">
-        <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
-      <c r="I42" s="10" t="s">
-        <v>117</v>
-      </c>
-      <c r="J42" s="10">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F42" s="7">
+        <v>10</v>
+      </c>
+      <c r="G42" s="7">
+        <v>1</v>
+      </c>
+      <c r="H42" s="7">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="I42" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="J42" s="7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A43" s="2">
         <v>40</v>
       </c>
@@ -2284,25 +2284,25 @@
       <c r="E43" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="F43" s="10">
-        <v>10</v>
-      </c>
-      <c r="G43" s="10">
-        <v>1</v>
-      </c>
-      <c r="H43" s="10">
-        <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
-      <c r="I43" s="10" t="s">
-        <v>117</v>
-      </c>
-      <c r="J43" s="10">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F43" s="7">
+        <v>10</v>
+      </c>
+      <c r="G43" s="7">
+        <v>1</v>
+      </c>
+      <c r="H43" s="7">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="I43" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="J43" s="7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A44" s="2">
         <v>41</v>
       </c>
@@ -2318,25 +2318,25 @@
       <c r="E44" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="F44" s="10">
-        <v>10</v>
-      </c>
-      <c r="G44" s="10">
-        <v>1</v>
-      </c>
-      <c r="H44" s="10">
-        <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
-      <c r="I44" s="10" t="s">
-        <v>117</v>
-      </c>
-      <c r="J44" s="10">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F44" s="7">
+        <v>10</v>
+      </c>
+      <c r="G44" s="7">
+        <v>1</v>
+      </c>
+      <c r="H44" s="7">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="I44" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="J44" s="7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A45" s="2">
         <v>42</v>
       </c>
@@ -2352,25 +2352,25 @@
       <c r="E45" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="F45" s="10">
-        <v>10</v>
-      </c>
-      <c r="G45" s="10">
-        <v>1</v>
-      </c>
-      <c r="H45" s="10">
-        <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
-      <c r="I45" s="10" t="s">
-        <v>117</v>
-      </c>
-      <c r="J45" s="10">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F45" s="7">
+        <v>10</v>
+      </c>
+      <c r="G45" s="7">
+        <v>1</v>
+      </c>
+      <c r="H45" s="7">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="I45" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="J45" s="7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A46" s="2">
         <v>43</v>
       </c>
@@ -2386,25 +2386,25 @@
       <c r="E46" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="F46" s="10">
-        <v>10</v>
-      </c>
-      <c r="G46" s="10">
-        <v>1</v>
-      </c>
-      <c r="H46" s="10">
-        <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
-      <c r="I46" s="10" t="s">
-        <v>117</v>
-      </c>
-      <c r="J46" s="10">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F46" s="7">
+        <v>10</v>
+      </c>
+      <c r="G46" s="7">
+        <v>1</v>
+      </c>
+      <c r="H46" s="7">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="I46" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="J46" s="7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A47" s="2">
         <v>44</v>
       </c>
@@ -2420,25 +2420,25 @@
       <c r="E47" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="F47" s="10">
-        <v>10</v>
-      </c>
-      <c r="G47" s="10">
-        <v>1</v>
-      </c>
-      <c r="H47" s="10">
-        <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
-      <c r="I47" s="10" t="s">
-        <v>117</v>
-      </c>
-      <c r="J47" s="10">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F47" s="7">
+        <v>10</v>
+      </c>
+      <c r="G47" s="7">
+        <v>1</v>
+      </c>
+      <c r="H47" s="7">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="I47" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="J47" s="7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A48" s="2">
         <v>45</v>
       </c>
@@ -2454,25 +2454,25 @@
       <c r="E48" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="F48" s="10">
-        <v>10</v>
-      </c>
-      <c r="G48" s="10">
-        <v>1</v>
-      </c>
-      <c r="H48" s="10">
-        <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
-      <c r="I48" s="10" t="s">
-        <v>117</v>
-      </c>
-      <c r="J48" s="10">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F48" s="7">
+        <v>10</v>
+      </c>
+      <c r="G48" s="7">
+        <v>1</v>
+      </c>
+      <c r="H48" s="7">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="I48" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="J48" s="7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A49" s="2">
         <v>46</v>
       </c>
@@ -2488,25 +2488,25 @@
       <c r="E49" s="5" t="s">
         <v>79</v>
       </c>
-      <c r="F49" s="10">
-        <v>10</v>
-      </c>
-      <c r="G49" s="10">
-        <v>1</v>
-      </c>
-      <c r="H49" s="10">
-        <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
-      <c r="I49" s="10" t="s">
-        <v>117</v>
-      </c>
-      <c r="J49" s="10">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F49" s="7">
+        <v>10</v>
+      </c>
+      <c r="G49" s="7">
+        <v>1</v>
+      </c>
+      <c r="H49" s="7">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="I49" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="J49" s="7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A50" s="2">
         <v>47</v>
       </c>
@@ -2522,25 +2522,25 @@
       <c r="E50" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="F50" s="10">
+      <c r="F50" s="7">
         <v>20</v>
       </c>
-      <c r="G50" s="10">
-        <v>1</v>
-      </c>
-      <c r="H50" s="10">
+      <c r="G50" s="7">
+        <v>1</v>
+      </c>
+      <c r="H50" s="7">
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
-      <c r="I50" s="10" t="s">
-        <v>117</v>
-      </c>
-      <c r="J50" s="10">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I50" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="J50" s="7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A51" s="2">
         <v>48</v>
       </c>
@@ -2556,25 +2556,25 @@
       <c r="E51" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="F51" s="10">
+      <c r="F51" s="7">
         <v>20</v>
       </c>
-      <c r="G51" s="10">
-        <v>1</v>
-      </c>
-      <c r="H51" s="10">
+      <c r="G51" s="7">
+        <v>1</v>
+      </c>
+      <c r="H51" s="7">
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
-      <c r="I51" s="10" t="s">
-        <v>117</v>
-      </c>
-      <c r="J51" s="10">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I51" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="J51" s="7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A52" s="2">
         <v>49</v>
       </c>
@@ -2590,25 +2590,25 @@
       <c r="E52" s="5" t="s">
         <v>107</v>
       </c>
-      <c r="F52" s="10">
+      <c r="F52" s="7">
         <v>20</v>
       </c>
-      <c r="G52" s="10">
-        <v>1</v>
-      </c>
-      <c r="H52" s="10">
+      <c r="G52" s="7">
+        <v>1</v>
+      </c>
+      <c r="H52" s="7">
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
-      <c r="I52" s="10" t="s">
-        <v>117</v>
-      </c>
-      <c r="J52" s="10">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I52" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="J52" s="7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A53" s="2">
         <v>50</v>
       </c>
@@ -2624,25 +2624,25 @@
       <c r="E53" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="F53" s="10">
+      <c r="F53" s="7">
         <v>20</v>
       </c>
-      <c r="G53" s="10">
-        <v>1</v>
-      </c>
-      <c r="H53" s="10">
+      <c r="G53" s="7">
+        <v>1</v>
+      </c>
+      <c r="H53" s="7">
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
-      <c r="I53" s="10" t="s">
-        <v>117</v>
-      </c>
-      <c r="J53" s="10">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I53" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="J53" s="7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A54" s="2">
         <v>51</v>
       </c>
@@ -2658,25 +2658,25 @@
       <c r="E54" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="F54" s="10">
+      <c r="F54" s="7">
         <v>20</v>
       </c>
-      <c r="G54" s="10">
-        <v>1</v>
-      </c>
-      <c r="H54" s="10">
+      <c r="G54" s="7">
+        <v>1</v>
+      </c>
+      <c r="H54" s="7">
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
-      <c r="I54" s="10" t="s">
-        <v>117</v>
-      </c>
-      <c r="J54" s="10">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I54" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="J54" s="7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A55" s="2">
         <v>52</v>
       </c>
@@ -2692,25 +2692,25 @@
       <c r="E55" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="F55" s="10">
+      <c r="F55" s="7">
         <v>20</v>
       </c>
-      <c r="G55" s="10">
-        <v>1</v>
-      </c>
-      <c r="H55" s="10">
+      <c r="G55" s="7">
+        <v>1</v>
+      </c>
+      <c r="H55" s="7">
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
-      <c r="I55" s="10" t="s">
-        <v>117</v>
-      </c>
-      <c r="J55" s="10">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I55" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="J55" s="7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A56" s="2">
         <v>53</v>
       </c>
@@ -2726,25 +2726,25 @@
       <c r="E56" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="F56" s="10">
+      <c r="F56" s="7">
         <v>20</v>
       </c>
-      <c r="G56" s="10">
-        <v>1</v>
-      </c>
-      <c r="H56" s="10">
+      <c r="G56" s="7">
+        <v>1</v>
+      </c>
+      <c r="H56" s="7">
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
-      <c r="I56" s="10" t="s">
-        <v>117</v>
-      </c>
-      <c r="J56" s="10">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I56" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="J56" s="7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A57" s="2">
         <v>54</v>
       </c>
@@ -2760,25 +2760,25 @@
       <c r="E57" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="F57" s="10">
+      <c r="F57" s="7">
         <v>20</v>
       </c>
-      <c r="G57" s="10">
-        <v>1</v>
-      </c>
-      <c r="H57" s="10">
+      <c r="G57" s="7">
+        <v>1</v>
+      </c>
+      <c r="H57" s="7">
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
-      <c r="I57" s="10" t="s">
-        <v>117</v>
-      </c>
-      <c r="J57" s="10">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I57" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="J57" s="7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A58" s="2">
         <v>55</v>
       </c>
@@ -2794,25 +2794,25 @@
       <c r="E58" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="F58" s="10">
+      <c r="F58" s="7">
         <v>20</v>
       </c>
-      <c r="G58" s="10">
-        <v>1</v>
-      </c>
-      <c r="H58" s="10">
+      <c r="G58" s="7">
+        <v>1</v>
+      </c>
+      <c r="H58" s="7">
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
-      <c r="I58" s="10" t="s">
-        <v>117</v>
-      </c>
-      <c r="J58" s="10">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I58" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="J58" s="7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A59" s="2">
         <v>56</v>
       </c>
@@ -2828,25 +2828,25 @@
       <c r="E59" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="F59" s="10">
-        <v>10</v>
-      </c>
-      <c r="G59" s="10">
-        <v>1</v>
-      </c>
-      <c r="H59" s="10">
-        <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
-      <c r="I59" s="10" t="s">
-        <v>117</v>
-      </c>
-      <c r="J59" s="10">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F59" s="7">
+        <v>10</v>
+      </c>
+      <c r="G59" s="7">
+        <v>1</v>
+      </c>
+      <c r="H59" s="7">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="I59" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="J59" s="7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A60" s="2">
         <v>57</v>
       </c>
@@ -2862,25 +2862,25 @@
       <c r="E60" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="F60" s="10">
-        <v>10</v>
-      </c>
-      <c r="G60" s="10">
-        <v>1</v>
-      </c>
-      <c r="H60" s="10">
-        <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
-      <c r="I60" s="10" t="s">
-        <v>117</v>
-      </c>
-      <c r="J60" s="10">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F60" s="7">
+        <v>10</v>
+      </c>
+      <c r="G60" s="7">
+        <v>1</v>
+      </c>
+      <c r="H60" s="7">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="I60" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="J60" s="7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A61" s="2">
         <v>58</v>
       </c>
@@ -2896,25 +2896,25 @@
       <c r="E61" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="F61" s="10">
-        <v>10</v>
-      </c>
-      <c r="G61" s="10">
-        <v>1</v>
-      </c>
-      <c r="H61" s="10">
-        <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
-      <c r="I61" s="10" t="s">
-        <v>117</v>
-      </c>
-      <c r="J61" s="10">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F61" s="7">
+        <v>10</v>
+      </c>
+      <c r="G61" s="7">
+        <v>1</v>
+      </c>
+      <c r="H61" s="7">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="I61" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="J61" s="7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A62" s="2">
         <v>59</v>
       </c>
@@ -2930,25 +2930,25 @@
       <c r="E62" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="F62" s="10">
-        <v>10</v>
-      </c>
-      <c r="G62" s="10">
-        <v>1</v>
-      </c>
-      <c r="H62" s="10">
-        <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
-      <c r="I62" s="10" t="s">
-        <v>117</v>
-      </c>
-      <c r="J62" s="10">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F62" s="7">
+        <v>10</v>
+      </c>
+      <c r="G62" s="7">
+        <v>1</v>
+      </c>
+      <c r="H62" s="7">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="I62" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="J62" s="7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A63" s="2">
         <v>60</v>
       </c>
@@ -2964,25 +2964,25 @@
       <c r="E63" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="F63" s="10">
-        <v>10</v>
-      </c>
-      <c r="G63" s="10">
-        <v>1</v>
-      </c>
-      <c r="H63" s="10">
-        <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
-      <c r="I63" s="10" t="s">
-        <v>117</v>
-      </c>
-      <c r="J63" s="10">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F63" s="7">
+        <v>10</v>
+      </c>
+      <c r="G63" s="7">
+        <v>1</v>
+      </c>
+      <c r="H63" s="7">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="I63" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="J63" s="7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A64" s="2">
         <v>61</v>
       </c>
@@ -2998,25 +2998,25 @@
       <c r="E64" s="5" t="s">
         <v>88</v>
       </c>
-      <c r="F64" s="10">
-        <v>10</v>
-      </c>
-      <c r="G64" s="10">
-        <v>1</v>
-      </c>
-      <c r="H64" s="10">
-        <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
-      <c r="I64" s="10" t="s">
-        <v>117</v>
-      </c>
-      <c r="J64" s="10">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="65" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F64" s="7">
+        <v>10</v>
+      </c>
+      <c r="G64" s="7">
+        <v>1</v>
+      </c>
+      <c r="H64" s="7">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="I64" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="J64" s="7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A65" s="2">
         <v>62</v>
       </c>
@@ -3032,25 +3032,25 @@
       <c r="E65" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="F65" s="10">
-        <v>10</v>
-      </c>
-      <c r="G65" s="10">
-        <v>1</v>
-      </c>
-      <c r="H65" s="10">
-        <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
-      <c r="I65" s="10" t="s">
-        <v>117</v>
-      </c>
-      <c r="J65" s="10">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="66" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F65" s="7">
+        <v>10</v>
+      </c>
+      <c r="G65" s="7">
+        <v>1</v>
+      </c>
+      <c r="H65" s="7">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="I65" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="J65" s="7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A66" s="2">
         <v>63</v>
       </c>
@@ -3066,25 +3066,25 @@
       <c r="E66" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="F66" s="10">
-        <v>10</v>
-      </c>
-      <c r="G66" s="10">
-        <v>1</v>
-      </c>
-      <c r="H66" s="10">
-        <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
-      <c r="I66" s="10" t="s">
-        <v>117</v>
-      </c>
-      <c r="J66" s="10">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F66" s="7">
+        <v>10</v>
+      </c>
+      <c r="G66" s="7">
+        <v>1</v>
+      </c>
+      <c r="H66" s="7">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="I66" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="J66" s="7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A67" s="2">
         <v>64</v>
       </c>
@@ -3100,25 +3100,25 @@
       <c r="E67" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="F67" s="10">
-        <v>10</v>
-      </c>
-      <c r="G67" s="10">
-        <v>1</v>
-      </c>
-      <c r="H67" s="10">
-        <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
-      <c r="I67" s="10" t="s">
-        <v>117</v>
-      </c>
-      <c r="J67" s="10">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F67" s="7">
+        <v>10</v>
+      </c>
+      <c r="G67" s="7">
+        <v>1</v>
+      </c>
+      <c r="H67" s="7">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="I67" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="J67" s="7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A68" s="2">
         <v>65</v>
       </c>
@@ -3134,25 +3134,25 @@
       <c r="E68" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="F68" s="10">
-        <v>10</v>
-      </c>
-      <c r="G68" s="10">
-        <v>1</v>
-      </c>
-      <c r="H68" s="10">
-        <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
-      <c r="I68" s="10" t="s">
-        <v>117</v>
-      </c>
-      <c r="J68" s="10">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F68" s="7">
+        <v>10</v>
+      </c>
+      <c r="G68" s="7">
+        <v>1</v>
+      </c>
+      <c r="H68" s="7">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="I68" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="J68" s="7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A69" s="2">
         <v>66</v>
       </c>
@@ -3168,25 +3168,25 @@
       <c r="E69" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="F69" s="10">
-        <v>10</v>
-      </c>
-      <c r="G69" s="10">
-        <v>1</v>
-      </c>
-      <c r="H69" s="10">
+      <c r="F69" s="7">
+        <v>10</v>
+      </c>
+      <c r="G69" s="7">
+        <v>1</v>
+      </c>
+      <c r="H69" s="7">
         <f t="shared" ref="H69:H103" si="2">F69*G69</f>
         <v>10</v>
       </c>
-      <c r="I69" s="10" t="s">
-        <v>117</v>
-      </c>
-      <c r="J69" s="10">
+      <c r="I69" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="J69" s="7">
         <f t="shared" ref="J69:J103" si="3">IF(I69="Finalizado",H69,0)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A70" s="2">
         <v>67</v>
       </c>
@@ -3202,25 +3202,25 @@
       <c r="E70" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="F70" s="10">
-        <v>10</v>
-      </c>
-      <c r="G70" s="10">
-        <v>1</v>
-      </c>
-      <c r="H70" s="10">
+      <c r="F70" s="7">
+        <v>10</v>
+      </c>
+      <c r="G70" s="7">
+        <v>1</v>
+      </c>
+      <c r="H70" s="7">
         <f t="shared" si="2"/>
         <v>10</v>
       </c>
-      <c r="I70" s="10" t="s">
-        <v>117</v>
-      </c>
-      <c r="J70" s="10">
+      <c r="I70" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="J70" s="7">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A71" s="2">
         <v>68</v>
       </c>
@@ -3236,25 +3236,25 @@
       <c r="E71" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="F71" s="10">
-        <v>10</v>
-      </c>
-      <c r="G71" s="10">
-        <v>1</v>
-      </c>
-      <c r="H71" s="10">
+      <c r="F71" s="7">
+        <v>10</v>
+      </c>
+      <c r="G71" s="7">
+        <v>1</v>
+      </c>
+      <c r="H71" s="7">
         <f t="shared" si="2"/>
         <v>10</v>
       </c>
-      <c r="I71" s="10" t="s">
-        <v>117</v>
-      </c>
-      <c r="J71" s="10">
+      <c r="I71" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="J71" s="7">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A72" s="2">
         <v>69</v>
       </c>
@@ -3270,25 +3270,25 @@
       <c r="E72" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="F72" s="10">
-        <v>10</v>
-      </c>
-      <c r="G72" s="10">
-        <v>1</v>
-      </c>
-      <c r="H72" s="10">
+      <c r="F72" s="7">
+        <v>10</v>
+      </c>
+      <c r="G72" s="7">
+        <v>1</v>
+      </c>
+      <c r="H72" s="7">
         <f t="shared" si="2"/>
         <v>10</v>
       </c>
-      <c r="I72" s="10" t="s">
-        <v>117</v>
-      </c>
-      <c r="J72" s="10">
+      <c r="I72" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="J72" s="7">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A73" s="2">
         <v>70</v>
       </c>
@@ -3304,25 +3304,25 @@
       <c r="E73" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="F73" s="10">
-        <v>10</v>
-      </c>
-      <c r="G73" s="10">
-        <v>1</v>
-      </c>
-      <c r="H73" s="10">
+      <c r="F73" s="7">
+        <v>10</v>
+      </c>
+      <c r="G73" s="7">
+        <v>1</v>
+      </c>
+      <c r="H73" s="7">
         <f t="shared" si="2"/>
         <v>10</v>
       </c>
-      <c r="I73" s="10" t="s">
-        <v>117</v>
-      </c>
-      <c r="J73" s="10">
+      <c r="I73" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="J73" s="7">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A74" s="2">
         <v>71</v>
       </c>
@@ -3338,25 +3338,25 @@
       <c r="E74" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="F74" s="10">
-        <v>10</v>
-      </c>
-      <c r="G74" s="10">
-        <v>1</v>
-      </c>
-      <c r="H74" s="10">
+      <c r="F74" s="7">
+        <v>10</v>
+      </c>
+      <c r="G74" s="7">
+        <v>1</v>
+      </c>
+      <c r="H74" s="7">
         <f t="shared" si="2"/>
         <v>10</v>
       </c>
-      <c r="I74" s="10" t="s">
-        <v>117</v>
-      </c>
-      <c r="J74" s="10">
+      <c r="I74" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="J74" s="7">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A75" s="2">
         <v>72</v>
       </c>
@@ -3372,25 +3372,25 @@
       <c r="E75" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="F75" s="10">
-        <v>10</v>
-      </c>
-      <c r="G75" s="10">
-        <v>1</v>
-      </c>
-      <c r="H75" s="10">
+      <c r="F75" s="7">
+        <v>10</v>
+      </c>
+      <c r="G75" s="7">
+        <v>1</v>
+      </c>
+      <c r="H75" s="7">
         <f t="shared" si="2"/>
         <v>10</v>
       </c>
-      <c r="I75" s="10" t="s">
-        <v>117</v>
-      </c>
-      <c r="J75" s="10">
+      <c r="I75" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="J75" s="7">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A76" s="2">
         <v>73</v>
       </c>
@@ -3406,25 +3406,25 @@
       <c r="E76" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="F76" s="10">
-        <v>10</v>
-      </c>
-      <c r="G76" s="10">
-        <v>1</v>
-      </c>
-      <c r="H76" s="10">
+      <c r="F76" s="7">
+        <v>10</v>
+      </c>
+      <c r="G76" s="7">
+        <v>1</v>
+      </c>
+      <c r="H76" s="7">
         <f t="shared" si="2"/>
         <v>10</v>
       </c>
-      <c r="I76" s="10" t="s">
-        <v>117</v>
-      </c>
-      <c r="J76" s="10">
+      <c r="I76" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="J76" s="7">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A77" s="2">
         <v>74</v>
       </c>
@@ -3440,25 +3440,25 @@
       <c r="E77" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="F77" s="10">
-        <v>10</v>
-      </c>
-      <c r="G77" s="10">
-        <v>1</v>
-      </c>
-      <c r="H77" s="10">
+      <c r="F77" s="7">
+        <v>10</v>
+      </c>
+      <c r="G77" s="7">
+        <v>1</v>
+      </c>
+      <c r="H77" s="7">
         <f t="shared" si="2"/>
         <v>10</v>
       </c>
-      <c r="I77" s="10" t="s">
-        <v>117</v>
-      </c>
-      <c r="J77" s="10">
+      <c r="I77" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="J77" s="7">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A78" s="2">
         <v>75</v>
       </c>
@@ -3474,25 +3474,25 @@
       <c r="E78" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="F78" s="10">
-        <v>10</v>
-      </c>
-      <c r="G78" s="10">
-        <v>1</v>
-      </c>
-      <c r="H78" s="10">
+      <c r="F78" s="7">
+        <v>10</v>
+      </c>
+      <c r="G78" s="7">
+        <v>1</v>
+      </c>
+      <c r="H78" s="7">
         <f t="shared" si="2"/>
         <v>10</v>
       </c>
-      <c r="I78" s="10" t="s">
-        <v>117</v>
-      </c>
-      <c r="J78" s="10">
+      <c r="I78" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="J78" s="7">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A79" s="2">
         <v>76</v>
       </c>
@@ -3508,25 +3508,25 @@
       <c r="E79" s="5" t="s">
         <v>110</v>
       </c>
-      <c r="F79" s="10">
+      <c r="F79" s="7">
         <v>90</v>
       </c>
-      <c r="G79" s="10">
+      <c r="G79" s="7">
         <v>34</v>
       </c>
-      <c r="H79" s="10">
+      <c r="H79" s="7">
         <f t="shared" si="2"/>
         <v>3060</v>
       </c>
-      <c r="I79" s="10" t="s">
-        <v>117</v>
-      </c>
-      <c r="J79" s="10">
+      <c r="I79" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="J79" s="7">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A80" s="2">
         <v>77</v>
       </c>
@@ -3542,25 +3542,25 @@
       <c r="E80" s="5" t="s">
         <v>86</v>
       </c>
-      <c r="F80" s="10">
+      <c r="F80" s="7">
         <v>90</v>
       </c>
-      <c r="G80" s="10">
-        <v>3</v>
-      </c>
-      <c r="H80" s="10">
+      <c r="G80" s="7">
+        <v>3</v>
+      </c>
+      <c r="H80" s="7">
         <f t="shared" si="2"/>
         <v>270</v>
       </c>
-      <c r="I80" s="10" t="s">
-        <v>117</v>
-      </c>
-      <c r="J80" s="10">
+      <c r="I80" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="J80" s="7">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
-    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A81" s="2">
         <v>78</v>
       </c>
@@ -3576,25 +3576,25 @@
       <c r="E81" s="5" t="s">
         <v>104</v>
       </c>
-      <c r="F81" s="10">
+      <c r="F81" s="7">
         <v>90</v>
       </c>
-      <c r="G81" s="10">
-        <v>3</v>
-      </c>
-      <c r="H81" s="10">
+      <c r="G81" s="7">
+        <v>3</v>
+      </c>
+      <c r="H81" s="7">
         <f t="shared" si="2"/>
         <v>270</v>
       </c>
-      <c r="I81" s="10" t="s">
-        <v>117</v>
-      </c>
-      <c r="J81" s="10">
+      <c r="I81" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="J81" s="7">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
-    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A82" s="2">
         <v>79</v>
       </c>
@@ -3610,25 +3610,25 @@
       <c r="E82" s="5" t="s">
         <v>90</v>
       </c>
-      <c r="F82" s="10">
+      <c r="F82" s="7">
         <v>90</v>
       </c>
-      <c r="G82" s="10">
-        <v>3</v>
-      </c>
-      <c r="H82" s="10">
+      <c r="G82" s="7">
+        <v>3</v>
+      </c>
+      <c r="H82" s="7">
         <f t="shared" si="2"/>
         <v>270</v>
       </c>
-      <c r="I82" s="10" t="s">
-        <v>117</v>
-      </c>
-      <c r="J82" s="10">
+      <c r="I82" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="J82" s="7">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A83" s="2">
         <v>80</v>
       </c>
@@ -3644,25 +3644,25 @@
       <c r="E83" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="F83" s="10">
-        <v>10</v>
-      </c>
-      <c r="G83" s="10">
+      <c r="F83" s="7">
+        <v>10</v>
+      </c>
+      <c r="G83" s="7">
         <v>5</v>
       </c>
-      <c r="H83" s="10">
+      <c r="H83" s="7">
         <f t="shared" si="2"/>
         <v>50</v>
       </c>
-      <c r="I83" s="10" t="s">
-        <v>117</v>
-      </c>
-      <c r="J83" s="10">
+      <c r="I83" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="J83" s="7">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A84" s="2">
         <v>81</v>
       </c>
@@ -3678,25 +3678,25 @@
       <c r="E84" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="F84" s="10">
-        <v>10</v>
-      </c>
-      <c r="G84" s="10">
+      <c r="F84" s="7">
+        <v>10</v>
+      </c>
+      <c r="G84" s="7">
         <v>5</v>
       </c>
-      <c r="H84" s="10">
+      <c r="H84" s="7">
         <f t="shared" si="2"/>
         <v>50</v>
       </c>
-      <c r="I84" s="10" t="s">
-        <v>117</v>
-      </c>
-      <c r="J84" s="10">
+      <c r="I84" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="J84" s="7">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
-    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A85" s="2">
         <v>82</v>
       </c>
@@ -3712,25 +3712,25 @@
       <c r="E85" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="F85" s="10">
-        <v>10</v>
-      </c>
-      <c r="G85" s="10">
+      <c r="F85" s="7">
+        <v>10</v>
+      </c>
+      <c r="G85" s="7">
         <v>21</v>
       </c>
-      <c r="H85" s="10">
+      <c r="H85" s="7">
         <f t="shared" si="2"/>
         <v>210</v>
       </c>
-      <c r="I85" s="10" t="s">
-        <v>117</v>
-      </c>
-      <c r="J85" s="10">
+      <c r="I85" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="J85" s="7">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A86" s="2">
         <v>83</v>
       </c>
@@ -3746,25 +3746,25 @@
       <c r="E86" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="F86" s="10">
-        <v>10</v>
-      </c>
-      <c r="G86" s="10">
+      <c r="F86" s="7">
+        <v>10</v>
+      </c>
+      <c r="G86" s="7">
         <v>21</v>
       </c>
-      <c r="H86" s="10">
+      <c r="H86" s="7">
         <f t="shared" si="2"/>
         <v>210</v>
       </c>
-      <c r="I86" s="10" t="s">
-        <v>117</v>
-      </c>
-      <c r="J86" s="10">
+      <c r="I86" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="J86" s="7">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
-    <row r="87" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A87" s="2">
         <v>84</v>
       </c>
@@ -3780,25 +3780,25 @@
       <c r="E87" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="F87" s="10">
-        <v>10</v>
-      </c>
-      <c r="G87" s="10">
+      <c r="F87" s="7">
+        <v>10</v>
+      </c>
+      <c r="G87" s="7">
         <v>21</v>
       </c>
-      <c r="H87" s="10">
+      <c r="H87" s="7">
         <f t="shared" si="2"/>
         <v>210</v>
       </c>
-      <c r="I87" s="10" t="s">
-        <v>117</v>
-      </c>
-      <c r="J87" s="10">
+      <c r="I87" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="J87" s="7">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
-    <row r="88" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A88" s="2">
         <v>85</v>
       </c>
@@ -3814,25 +3814,25 @@
       <c r="E88" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="F88" s="10">
+      <c r="F88" s="7">
         <v>60</v>
       </c>
-      <c r="G88" s="10">
-        <v>3</v>
-      </c>
-      <c r="H88" s="10">
+      <c r="G88" s="7">
+        <v>3</v>
+      </c>
+      <c r="H88" s="7">
         <f t="shared" si="2"/>
         <v>180</v>
       </c>
-      <c r="I88" s="10" t="s">
-        <v>117</v>
-      </c>
-      <c r="J88" s="10">
+      <c r="I88" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="J88" s="7">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
-    <row r="89" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A89" s="2">
         <v>86</v>
       </c>
@@ -3848,25 +3848,25 @@
       <c r="E89" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="F89" s="10">
+      <c r="F89" s="7">
         <v>60</v>
       </c>
-      <c r="G89" s="10">
-        <v>3</v>
-      </c>
-      <c r="H89" s="10">
+      <c r="G89" s="7">
+        <v>3</v>
+      </c>
+      <c r="H89" s="7">
         <f t="shared" si="2"/>
         <v>180</v>
       </c>
-      <c r="I89" s="10" t="s">
-        <v>117</v>
-      </c>
-      <c r="J89" s="10">
+      <c r="I89" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="J89" s="7">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
-    <row r="90" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A90" s="2">
         <v>87</v>
       </c>
@@ -3882,25 +3882,25 @@
       <c r="E90" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="F90" s="10">
+      <c r="F90" s="7">
         <v>60</v>
       </c>
-      <c r="G90" s="10">
-        <v>3</v>
-      </c>
-      <c r="H90" s="10">
+      <c r="G90" s="7">
+        <v>3</v>
+      </c>
+      <c r="H90" s="7">
         <f t="shared" si="2"/>
         <v>180</v>
       </c>
-      <c r="I90" s="10" t="s">
-        <v>117</v>
-      </c>
-      <c r="J90" s="10">
+      <c r="I90" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="J90" s="7">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
-    <row r="91" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A91" s="2">
         <v>88</v>
       </c>
@@ -3916,25 +3916,25 @@
       <c r="E91" s="5" t="s">
         <v>98</v>
       </c>
-      <c r="F91" s="10">
+      <c r="F91" s="7">
         <v>60</v>
       </c>
-      <c r="G91" s="10">
-        <v>3</v>
-      </c>
-      <c r="H91" s="10">
+      <c r="G91" s="7">
+        <v>3</v>
+      </c>
+      <c r="H91" s="7">
         <f t="shared" si="2"/>
         <v>180</v>
       </c>
-      <c r="I91" s="10" t="s">
-        <v>117</v>
-      </c>
-      <c r="J91" s="10">
+      <c r="I91" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="J91" s="7">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
-    <row r="92" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A92" s="2">
         <v>89</v>
       </c>
@@ -3950,25 +3950,25 @@
       <c r="E92" s="5" t="s">
         <v>99</v>
       </c>
-      <c r="F92" s="10">
+      <c r="F92" s="7">
         <v>60</v>
       </c>
-      <c r="G92" s="10">
-        <v>3</v>
-      </c>
-      <c r="H92" s="10">
+      <c r="G92" s="7">
+        <v>3</v>
+      </c>
+      <c r="H92" s="7">
         <f t="shared" si="2"/>
         <v>180</v>
       </c>
-      <c r="I92" s="10" t="s">
-        <v>117</v>
-      </c>
-      <c r="J92" s="10">
+      <c r="I92" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="J92" s="7">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
-    <row r="93" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A93" s="2">
         <v>90</v>
       </c>
@@ -3984,25 +3984,25 @@
       <c r="E93" s="5" t="s">
         <v>100</v>
       </c>
-      <c r="F93" s="10">
+      <c r="F93" s="7">
         <v>60</v>
       </c>
-      <c r="G93" s="10">
-        <v>3</v>
-      </c>
-      <c r="H93" s="10">
+      <c r="G93" s="7">
+        <v>3</v>
+      </c>
+      <c r="H93" s="7">
         <f t="shared" si="2"/>
         <v>180</v>
       </c>
-      <c r="I93" s="10" t="s">
-        <v>117</v>
-      </c>
-      <c r="J93" s="10">
+      <c r="I93" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="J93" s="7">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
-    <row r="94" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A94" s="2">
         <v>91</v>
       </c>
@@ -4018,25 +4018,25 @@
       <c r="E94" s="5" t="s">
         <v>101</v>
       </c>
-      <c r="F94" s="10">
+      <c r="F94" s="7">
         <v>60</v>
       </c>
-      <c r="G94" s="10">
-        <v>3</v>
-      </c>
-      <c r="H94" s="10">
+      <c r="G94" s="7">
+        <v>3</v>
+      </c>
+      <c r="H94" s="7">
         <f t="shared" si="2"/>
         <v>180</v>
       </c>
-      <c r="I94" s="10" t="s">
-        <v>117</v>
-      </c>
-      <c r="J94" s="10">
+      <c r="I94" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="J94" s="7">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
-    <row r="95" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A95" s="2">
         <v>92</v>
       </c>
@@ -4052,25 +4052,25 @@
       <c r="E95" s="5" t="s">
         <v>102</v>
       </c>
-      <c r="F95" s="10">
+      <c r="F95" s="7">
         <v>60</v>
       </c>
-      <c r="G95" s="10">
-        <v>3</v>
-      </c>
-      <c r="H95" s="10">
+      <c r="G95" s="7">
+        <v>3</v>
+      </c>
+      <c r="H95" s="7">
         <f t="shared" si="2"/>
         <v>180</v>
       </c>
-      <c r="I95" s="10" t="s">
-        <v>117</v>
-      </c>
-      <c r="J95" s="10">
+      <c r="I95" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="J95" s="7">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
-    <row r="96" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A96" s="2">
         <v>93</v>
       </c>
@@ -4086,25 +4086,25 @@
       <c r="E96" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="F96" s="10">
-        <v>10</v>
-      </c>
-      <c r="G96" s="10">
-        <v>3</v>
-      </c>
-      <c r="H96" s="10">
+      <c r="F96" s="7">
+        <v>10</v>
+      </c>
+      <c r="G96" s="7">
+        <v>3</v>
+      </c>
+      <c r="H96" s="7">
         <f t="shared" si="2"/>
         <v>30</v>
       </c>
-      <c r="I96" s="10" t="s">
-        <v>117</v>
-      </c>
-      <c r="J96" s="10">
+      <c r="I96" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="J96" s="7">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
-    <row r="97" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A97" s="2">
         <v>94</v>
       </c>
@@ -4120,25 +4120,25 @@
       <c r="E97" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="F97" s="10">
-        <v>10</v>
-      </c>
-      <c r="G97" s="10">
-        <v>3</v>
-      </c>
-      <c r="H97" s="10">
+      <c r="F97" s="7">
+        <v>10</v>
+      </c>
+      <c r="G97" s="7">
+        <v>3</v>
+      </c>
+      <c r="H97" s="7">
         <f t="shared" si="2"/>
         <v>30</v>
       </c>
-      <c r="I97" s="10" t="s">
-        <v>117</v>
-      </c>
-      <c r="J97" s="10">
+      <c r="I97" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="J97" s="7">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
-    <row r="98" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A98" s="2">
         <v>95</v>
       </c>
@@ -4154,25 +4154,25 @@
       <c r="E98" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="F98" s="10">
-        <v>10</v>
-      </c>
-      <c r="G98" s="10">
-        <v>3</v>
-      </c>
-      <c r="H98" s="10">
+      <c r="F98" s="7">
+        <v>10</v>
+      </c>
+      <c r="G98" s="7">
+        <v>3</v>
+      </c>
+      <c r="H98" s="7">
         <f t="shared" si="2"/>
         <v>30</v>
       </c>
-      <c r="I98" s="10" t="s">
-        <v>117</v>
-      </c>
-      <c r="J98" s="10">
+      <c r="I98" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="J98" s="7">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
-    <row r="99" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A99" s="2">
         <v>96</v>
       </c>
@@ -4188,25 +4188,25 @@
       <c r="E99" s="5" t="s">
         <v>92</v>
       </c>
-      <c r="F99" s="10">
-        <v>10</v>
-      </c>
-      <c r="G99" s="10">
+      <c r="F99" s="7">
+        <v>10</v>
+      </c>
+      <c r="G99" s="7">
         <v>5</v>
       </c>
-      <c r="H99" s="10">
+      <c r="H99" s="7">
         <f t="shared" si="2"/>
         <v>50</v>
       </c>
-      <c r="I99" s="10" t="s">
-        <v>117</v>
-      </c>
-      <c r="J99" s="10">
+      <c r="I99" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="J99" s="7">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
-    <row r="100" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A100" s="2">
         <v>97</v>
       </c>
@@ -4222,25 +4222,25 @@
       <c r="E100" s="5" t="s">
         <v>93</v>
       </c>
-      <c r="F100" s="10">
-        <v>10</v>
-      </c>
-      <c r="G100" s="10">
-        <v>3</v>
-      </c>
-      <c r="H100" s="10">
+      <c r="F100" s="7">
+        <v>10</v>
+      </c>
+      <c r="G100" s="7">
+        <v>3</v>
+      </c>
+      <c r="H100" s="7">
         <f t="shared" si="2"/>
         <v>30</v>
       </c>
-      <c r="I100" s="10" t="s">
-        <v>117</v>
-      </c>
-      <c r="J100" s="10">
+      <c r="I100" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="J100" s="7">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
-    <row r="101" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A101" s="2">
         <v>98</v>
       </c>
@@ -4256,25 +4256,25 @@
       <c r="E101" s="5" t="s">
         <v>94</v>
       </c>
-      <c r="F101" s="10">
-        <v>10</v>
-      </c>
-      <c r="G101" s="10">
-        <v>3</v>
-      </c>
-      <c r="H101" s="10">
+      <c r="F101" s="7">
+        <v>10</v>
+      </c>
+      <c r="G101" s="7">
+        <v>3</v>
+      </c>
+      <c r="H101" s="7">
         <f t="shared" si="2"/>
         <v>30</v>
       </c>
-      <c r="I101" s="10" t="s">
-        <v>117</v>
-      </c>
-      <c r="J101" s="10">
+      <c r="I101" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="J101" s="7">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
-    <row r="102" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A102" s="2">
         <v>99</v>
       </c>
@@ -4290,25 +4290,25 @@
       <c r="E102" s="5" t="s">
         <v>95</v>
       </c>
-      <c r="F102" s="10">
-        <v>10</v>
-      </c>
-      <c r="G102" s="10">
+      <c r="F102" s="7">
+        <v>10</v>
+      </c>
+      <c r="G102" s="7">
         <v>13</v>
       </c>
-      <c r="H102" s="10">
+      <c r="H102" s="7">
         <f t="shared" si="2"/>
         <v>130</v>
       </c>
-      <c r="I102" s="10" t="s">
-        <v>117</v>
-      </c>
-      <c r="J102" s="10">
+      <c r="I102" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="J102" s="7">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
-    <row r="103" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A103" s="2">
         <v>100</v>
       </c>
@@ -4324,28 +4324,28 @@
       <c r="E103" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="F103" s="10">
-        <v>10</v>
-      </c>
-      <c r="G103" s="10">
+      <c r="F103" s="7">
+        <v>10</v>
+      </c>
+      <c r="G103" s="7">
         <v>13</v>
       </c>
-      <c r="H103" s="10">
+      <c r="H103" s="7">
         <f t="shared" si="2"/>
         <v>130</v>
       </c>
-      <c r="I103" s="10" t="s">
-        <v>117</v>
-      </c>
-      <c r="J103" s="10">
+      <c r="I103" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="J103" s="7">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
-    <row r="104" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:10" x14ac:dyDescent="0.3">
       <c r="E104" s="4"/>
     </row>
-    <row r="144" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="144" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E144" s="3"/>
     </row>
   </sheetData>
@@ -4388,19 +4388,19 @@
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>115</v>
       </c>

</xml_diff>